<commit_message>
Completed pg. 178 data entry for "Frequency of Capture"
</commit_message>
<xml_diff>
--- a/Lovejoy data table_Frequency of capture.xlsx
+++ b/Lovejoy data table_Frequency of capture.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="15">
   <si>
     <t>Bird Species</t>
   </si>
@@ -404,9 +404,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CB20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3809,6 +3809,237 @@
       <c r="C15">
         <v>11</v>
       </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>1</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>0</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>1</v>
+      </c>
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15">
+        <v>1</v>
+      </c>
+      <c r="AD15">
+        <v>0</v>
+      </c>
+      <c r="AE15">
+        <v>0</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>0</v>
+      </c>
+      <c r="AH15">
+        <v>0</v>
+      </c>
+      <c r="AI15">
+        <v>0</v>
+      </c>
+      <c r="AJ15">
+        <v>0</v>
+      </c>
+      <c r="AK15">
+        <v>1</v>
+      </c>
+      <c r="AL15">
+        <v>1</v>
+      </c>
+      <c r="AM15">
+        <v>0</v>
+      </c>
+      <c r="AN15">
+        <v>1</v>
+      </c>
+      <c r="AO15">
+        <v>0</v>
+      </c>
+      <c r="AP15">
+        <v>0</v>
+      </c>
+      <c r="AQ15">
+        <v>0</v>
+      </c>
+      <c r="AR15">
+        <v>0</v>
+      </c>
+      <c r="AS15">
+        <v>0</v>
+      </c>
+      <c r="AT15">
+        <v>0</v>
+      </c>
+      <c r="AU15">
+        <v>1</v>
+      </c>
+      <c r="AV15">
+        <v>0</v>
+      </c>
+      <c r="AW15">
+        <v>0</v>
+      </c>
+      <c r="AX15">
+        <v>0</v>
+      </c>
+      <c r="AY15">
+        <v>0</v>
+      </c>
+      <c r="AZ15">
+        <v>0</v>
+      </c>
+      <c r="BA15">
+        <v>0</v>
+      </c>
+      <c r="BB15">
+        <v>0</v>
+      </c>
+      <c r="BC15">
+        <v>0</v>
+      </c>
+      <c r="BD15">
+        <v>0</v>
+      </c>
+      <c r="BE15">
+        <v>0</v>
+      </c>
+      <c r="BF15">
+        <v>0</v>
+      </c>
+      <c r="BG15">
+        <v>0</v>
+      </c>
+      <c r="BH15">
+        <v>0</v>
+      </c>
+      <c r="BI15">
+        <v>1</v>
+      </c>
+      <c r="BJ15">
+        <v>0</v>
+      </c>
+      <c r="BK15">
+        <v>0</v>
+      </c>
+      <c r="BL15">
+        <v>0</v>
+      </c>
+      <c r="BM15">
+        <v>0</v>
+      </c>
+      <c r="BN15">
+        <v>0</v>
+      </c>
+      <c r="BO15">
+        <v>0</v>
+      </c>
+      <c r="BP15">
+        <v>0</v>
+      </c>
+      <c r="BQ15">
+        <v>0</v>
+      </c>
+      <c r="BR15">
+        <v>1</v>
+      </c>
+      <c r="BS15">
+        <v>0</v>
+      </c>
+      <c r="BT15">
+        <v>1</v>
+      </c>
+      <c r="BU15">
+        <v>0</v>
+      </c>
+      <c r="BV15" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW15">
+        <v>0</v>
+      </c>
+      <c r="BX15" t="s">
+        <v>7</v>
+      </c>
+      <c r="BY15">
+        <v>0</v>
+      </c>
+      <c r="BZ15">
+        <v>0</v>
+      </c>
+      <c r="CA15">
+        <v>0</v>
+      </c>
+      <c r="CB15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -3820,8 +4051,239 @@
       <c r="C16">
         <v>0</v>
       </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16">
+        <v>0</v>
+      </c>
+      <c r="AD16">
+        <v>0</v>
+      </c>
+      <c r="AE16">
+        <v>0</v>
+      </c>
+      <c r="AF16">
+        <v>0</v>
+      </c>
+      <c r="AG16">
+        <v>0</v>
+      </c>
+      <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16">
+        <v>0</v>
+      </c>
+      <c r="AJ16">
+        <v>0</v>
+      </c>
+      <c r="AK16">
+        <v>0</v>
+      </c>
+      <c r="AL16">
+        <v>0</v>
+      </c>
+      <c r="AM16">
+        <v>0</v>
+      </c>
+      <c r="AN16">
+        <v>0</v>
+      </c>
+      <c r="AO16">
+        <v>0</v>
+      </c>
+      <c r="AP16">
+        <v>0</v>
+      </c>
+      <c r="AQ16">
+        <v>0</v>
+      </c>
+      <c r="AR16">
+        <v>0</v>
+      </c>
+      <c r="AS16">
+        <v>0</v>
+      </c>
+      <c r="AT16">
+        <v>0</v>
+      </c>
+      <c r="AU16">
+        <v>0</v>
+      </c>
+      <c r="AV16">
+        <v>0</v>
+      </c>
+      <c r="AW16">
+        <v>0</v>
+      </c>
+      <c r="AX16">
+        <v>0</v>
+      </c>
+      <c r="AY16">
+        <v>0</v>
+      </c>
+      <c r="AZ16">
+        <v>0</v>
+      </c>
+      <c r="BA16">
+        <v>0</v>
+      </c>
+      <c r="BB16">
+        <v>0</v>
+      </c>
+      <c r="BC16">
+        <v>0</v>
+      </c>
+      <c r="BD16">
+        <v>0</v>
+      </c>
+      <c r="BE16">
+        <v>0</v>
+      </c>
+      <c r="BF16">
+        <v>0</v>
+      </c>
+      <c r="BG16">
+        <v>0</v>
+      </c>
+      <c r="BH16">
+        <v>0</v>
+      </c>
+      <c r="BI16">
+        <v>0</v>
+      </c>
+      <c r="BJ16">
+        <v>0</v>
+      </c>
+      <c r="BK16">
+        <v>0</v>
+      </c>
+      <c r="BL16">
+        <v>0</v>
+      </c>
+      <c r="BM16">
+        <v>0</v>
+      </c>
+      <c r="BN16">
+        <v>0</v>
+      </c>
+      <c r="BO16">
+        <v>0</v>
+      </c>
+      <c r="BP16">
+        <v>0</v>
+      </c>
+      <c r="BQ16">
+        <v>0</v>
+      </c>
+      <c r="BR16">
+        <v>0</v>
+      </c>
+      <c r="BS16">
+        <v>0</v>
+      </c>
+      <c r="BT16">
+        <v>0</v>
+      </c>
+      <c r="BU16">
+        <v>0</v>
+      </c>
+      <c r="BV16">
+        <v>0</v>
+      </c>
+      <c r="BW16">
+        <v>0</v>
+      </c>
+      <c r="BX16">
+        <v>0</v>
+      </c>
+      <c r="BY16">
+        <v>0</v>
+      </c>
+      <c r="BZ16">
+        <v>0</v>
+      </c>
+      <c r="CA16">
+        <v>0</v>
+      </c>
+      <c r="CB16">
+        <v>0</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>139</v>
       </c>
@@ -3831,8 +4293,239 @@
       <c r="C17">
         <v>33</v>
       </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>1</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>1</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>0</v>
+      </c>
+      <c r="W17">
+        <v>1</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>1</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>1</v>
+      </c>
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17">
+        <v>0</v>
+      </c>
+      <c r="AD17">
+        <v>0</v>
+      </c>
+      <c r="AE17">
+        <v>0</v>
+      </c>
+      <c r="AF17">
+        <v>1</v>
+      </c>
+      <c r="AG17">
+        <v>1</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>7</v>
+      </c>
+      <c r="AI17">
+        <v>0</v>
+      </c>
+      <c r="AJ17">
+        <v>0</v>
+      </c>
+      <c r="AK17">
+        <v>0</v>
+      </c>
+      <c r="AL17">
+        <v>0</v>
+      </c>
+      <c r="AM17">
+        <v>0</v>
+      </c>
+      <c r="AN17">
+        <v>0</v>
+      </c>
+      <c r="AO17">
+        <v>0</v>
+      </c>
+      <c r="AP17">
+        <v>0</v>
+      </c>
+      <c r="AQ17">
+        <v>0</v>
+      </c>
+      <c r="AR17">
+        <v>1</v>
+      </c>
+      <c r="AS17">
+        <v>1</v>
+      </c>
+      <c r="AT17">
+        <v>1</v>
+      </c>
+      <c r="AU17">
+        <v>1</v>
+      </c>
+      <c r="AV17">
+        <v>1</v>
+      </c>
+      <c r="AW17">
+        <v>2</v>
+      </c>
+      <c r="AX17">
+        <v>0</v>
+      </c>
+      <c r="AY17">
+        <v>1</v>
+      </c>
+      <c r="AZ17">
+        <v>0</v>
+      </c>
+      <c r="BA17">
+        <v>3</v>
+      </c>
+      <c r="BB17">
+        <v>2</v>
+      </c>
+      <c r="BC17">
+        <v>0</v>
+      </c>
+      <c r="BD17">
+        <v>0</v>
+      </c>
+      <c r="BE17">
+        <v>0</v>
+      </c>
+      <c r="BF17">
+        <v>2</v>
+      </c>
+      <c r="BG17">
+        <v>0</v>
+      </c>
+      <c r="BH17">
+        <v>0</v>
+      </c>
+      <c r="BI17">
+        <v>0</v>
+      </c>
+      <c r="BJ17">
+        <v>0</v>
+      </c>
+      <c r="BK17">
+        <v>0</v>
+      </c>
+      <c r="BL17">
+        <v>0</v>
+      </c>
+      <c r="BM17">
+        <v>0</v>
+      </c>
+      <c r="BN17">
+        <v>0</v>
+      </c>
+      <c r="BO17">
+        <v>1</v>
+      </c>
+      <c r="BP17">
+        <v>0</v>
+      </c>
+      <c r="BQ17">
+        <v>0</v>
+      </c>
+      <c r="BR17">
+        <v>0</v>
+      </c>
+      <c r="BS17">
+        <v>0</v>
+      </c>
+      <c r="BT17">
+        <v>0</v>
+      </c>
+      <c r="BU17">
+        <v>0</v>
+      </c>
+      <c r="BV17">
+        <v>0</v>
+      </c>
+      <c r="BW17">
+        <v>0</v>
+      </c>
+      <c r="BX17">
+        <v>1</v>
+      </c>
+      <c r="BY17">
+        <v>1</v>
+      </c>
+      <c r="BZ17">
+        <v>1</v>
+      </c>
+      <c r="CA17">
+        <v>0</v>
+      </c>
+      <c r="CB17">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>140</v>
       </c>
@@ -3842,8 +4535,239 @@
       <c r="C18">
         <v>2</v>
       </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>0</v>
+      </c>
+      <c r="T18">
+        <v>0</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18">
+        <v>0</v>
+      </c>
+      <c r="AD18">
+        <v>0</v>
+      </c>
+      <c r="AE18">
+        <v>0</v>
+      </c>
+      <c r="AF18">
+        <v>0</v>
+      </c>
+      <c r="AG18">
+        <v>0</v>
+      </c>
+      <c r="AH18">
+        <v>0</v>
+      </c>
+      <c r="AI18">
+        <v>0</v>
+      </c>
+      <c r="AJ18">
+        <v>0</v>
+      </c>
+      <c r="AK18">
+        <v>0</v>
+      </c>
+      <c r="AL18">
+        <v>0</v>
+      </c>
+      <c r="AM18">
+        <v>0</v>
+      </c>
+      <c r="AN18">
+        <v>0</v>
+      </c>
+      <c r="AO18">
+        <v>0</v>
+      </c>
+      <c r="AP18">
+        <v>0</v>
+      </c>
+      <c r="AQ18">
+        <v>0</v>
+      </c>
+      <c r="AR18">
+        <v>0</v>
+      </c>
+      <c r="AS18">
+        <v>1</v>
+      </c>
+      <c r="AT18">
+        <v>0</v>
+      </c>
+      <c r="AU18">
+        <v>0</v>
+      </c>
+      <c r="AV18">
+        <v>0</v>
+      </c>
+      <c r="AW18">
+        <v>0</v>
+      </c>
+      <c r="AX18">
+        <v>0</v>
+      </c>
+      <c r="AY18">
+        <v>0</v>
+      </c>
+      <c r="AZ18">
+        <v>0</v>
+      </c>
+      <c r="BA18">
+        <v>0</v>
+      </c>
+      <c r="BB18">
+        <v>0</v>
+      </c>
+      <c r="BC18">
+        <v>0</v>
+      </c>
+      <c r="BD18">
+        <v>0</v>
+      </c>
+      <c r="BE18">
+        <v>0</v>
+      </c>
+      <c r="BF18">
+        <v>0</v>
+      </c>
+      <c r="BG18">
+        <v>0</v>
+      </c>
+      <c r="BH18">
+        <v>0</v>
+      </c>
+      <c r="BI18">
+        <v>0</v>
+      </c>
+      <c r="BJ18">
+        <v>0</v>
+      </c>
+      <c r="BK18">
+        <v>0</v>
+      </c>
+      <c r="BL18">
+        <v>0</v>
+      </c>
+      <c r="BM18">
+        <v>0</v>
+      </c>
+      <c r="BN18">
+        <v>0</v>
+      </c>
+      <c r="BO18">
+        <v>0</v>
+      </c>
+      <c r="BP18">
+        <v>0</v>
+      </c>
+      <c r="BQ18">
+        <v>0</v>
+      </c>
+      <c r="BR18">
+        <v>0</v>
+      </c>
+      <c r="BS18">
+        <v>0</v>
+      </c>
+      <c r="BT18">
+        <v>0</v>
+      </c>
+      <c r="BU18">
+        <v>0</v>
+      </c>
+      <c r="BV18" t="s">
+        <v>7</v>
+      </c>
+      <c r="BW18">
+        <v>0</v>
+      </c>
+      <c r="BX18">
+        <v>0</v>
+      </c>
+      <c r="BY18">
+        <v>0</v>
+      </c>
+      <c r="BZ18">
+        <v>0</v>
+      </c>
+      <c r="CA18">
+        <v>0</v>
+      </c>
+      <c r="CB18">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>142</v>
       </c>
@@ -3853,8 +4777,239 @@
       <c r="C19">
         <v>8</v>
       </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>0</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>2</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19">
+        <v>0</v>
+      </c>
+      <c r="AD19">
+        <v>0</v>
+      </c>
+      <c r="AE19">
+        <v>0</v>
+      </c>
+      <c r="AF19">
+        <v>0</v>
+      </c>
+      <c r="AG19">
+        <v>0</v>
+      </c>
+      <c r="AH19">
+        <v>0</v>
+      </c>
+      <c r="AI19">
+        <v>0</v>
+      </c>
+      <c r="AJ19">
+        <v>0</v>
+      </c>
+      <c r="AK19">
+        <v>0</v>
+      </c>
+      <c r="AL19">
+        <v>0</v>
+      </c>
+      <c r="AM19">
+        <v>0</v>
+      </c>
+      <c r="AN19">
+        <v>0</v>
+      </c>
+      <c r="AO19">
+        <v>1</v>
+      </c>
+      <c r="AP19">
+        <v>0</v>
+      </c>
+      <c r="AQ19">
+        <v>0</v>
+      </c>
+      <c r="AR19">
+        <v>0</v>
+      </c>
+      <c r="AS19">
+        <v>0</v>
+      </c>
+      <c r="AT19">
+        <v>0</v>
+      </c>
+      <c r="AU19">
+        <v>0</v>
+      </c>
+      <c r="AV19">
+        <v>0</v>
+      </c>
+      <c r="AW19">
+        <v>0</v>
+      </c>
+      <c r="AX19">
+        <v>0</v>
+      </c>
+      <c r="AY19">
+        <v>0</v>
+      </c>
+      <c r="AZ19">
+        <v>0</v>
+      </c>
+      <c r="BA19">
+        <v>0</v>
+      </c>
+      <c r="BB19">
+        <v>0</v>
+      </c>
+      <c r="BC19">
+        <v>0</v>
+      </c>
+      <c r="BD19">
+        <v>0</v>
+      </c>
+      <c r="BE19">
+        <v>0</v>
+      </c>
+      <c r="BF19">
+        <v>0</v>
+      </c>
+      <c r="BG19">
+        <v>0</v>
+      </c>
+      <c r="BH19">
+        <v>0</v>
+      </c>
+      <c r="BI19">
+        <v>0</v>
+      </c>
+      <c r="BJ19">
+        <v>0</v>
+      </c>
+      <c r="BK19">
+        <v>0</v>
+      </c>
+      <c r="BL19">
+        <v>0</v>
+      </c>
+      <c r="BM19">
+        <v>0</v>
+      </c>
+      <c r="BN19">
+        <v>0</v>
+      </c>
+      <c r="BO19">
+        <v>0</v>
+      </c>
+      <c r="BP19">
+        <v>0</v>
+      </c>
+      <c r="BQ19">
+        <v>0</v>
+      </c>
+      <c r="BR19">
+        <v>0</v>
+      </c>
+      <c r="BS19">
+        <v>0</v>
+      </c>
+      <c r="BT19">
+        <v>0</v>
+      </c>
+      <c r="BU19">
+        <v>0</v>
+      </c>
+      <c r="BV19">
+        <v>0</v>
+      </c>
+      <c r="BW19">
+        <v>0</v>
+      </c>
+      <c r="BX19">
+        <v>0</v>
+      </c>
+      <c r="BY19">
+        <v>0</v>
+      </c>
+      <c r="BZ19">
+        <v>0</v>
+      </c>
+      <c r="CA19">
+        <v>0</v>
+      </c>
+      <c r="CB19">
+        <v>0</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>143</v>
       </c>
@@ -3863,6 +5018,237 @@
       </c>
       <c r="C20">
         <v>1</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>0</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>0</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+      <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20">
+        <v>0</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <v>0</v>
+      </c>
+      <c r="AF20">
+        <v>0</v>
+      </c>
+      <c r="AG20">
+        <v>0</v>
+      </c>
+      <c r="AH20">
+        <v>0</v>
+      </c>
+      <c r="AI20">
+        <v>0</v>
+      </c>
+      <c r="AJ20">
+        <v>0</v>
+      </c>
+      <c r="AK20">
+        <v>0</v>
+      </c>
+      <c r="AL20">
+        <v>0</v>
+      </c>
+      <c r="AM20">
+        <v>0</v>
+      </c>
+      <c r="AN20">
+        <v>0</v>
+      </c>
+      <c r="AO20">
+        <v>0</v>
+      </c>
+      <c r="AP20">
+        <v>0</v>
+      </c>
+      <c r="AQ20">
+        <v>0</v>
+      </c>
+      <c r="AR20">
+        <v>0</v>
+      </c>
+      <c r="AS20">
+        <v>0</v>
+      </c>
+      <c r="AT20">
+        <v>0</v>
+      </c>
+      <c r="AU20">
+        <v>0</v>
+      </c>
+      <c r="AV20">
+        <v>0</v>
+      </c>
+      <c r="AW20">
+        <v>0</v>
+      </c>
+      <c r="AX20">
+        <v>0</v>
+      </c>
+      <c r="AY20">
+        <v>0</v>
+      </c>
+      <c r="AZ20">
+        <v>0</v>
+      </c>
+      <c r="BA20">
+        <v>0</v>
+      </c>
+      <c r="BB20">
+        <v>0</v>
+      </c>
+      <c r="BC20">
+        <v>0</v>
+      </c>
+      <c r="BD20">
+        <v>0</v>
+      </c>
+      <c r="BE20">
+        <v>0</v>
+      </c>
+      <c r="BF20">
+        <v>0</v>
+      </c>
+      <c r="BG20">
+        <v>0</v>
+      </c>
+      <c r="BH20">
+        <v>0</v>
+      </c>
+      <c r="BI20">
+        <v>0</v>
+      </c>
+      <c r="BJ20">
+        <v>0</v>
+      </c>
+      <c r="BK20">
+        <v>0</v>
+      </c>
+      <c r="BL20">
+        <v>0</v>
+      </c>
+      <c r="BM20">
+        <v>0</v>
+      </c>
+      <c r="BN20">
+        <v>0</v>
+      </c>
+      <c r="BO20">
+        <v>0</v>
+      </c>
+      <c r="BP20">
+        <v>0</v>
+      </c>
+      <c r="BQ20">
+        <v>0</v>
+      </c>
+      <c r="BR20">
+        <v>0</v>
+      </c>
+      <c r="BS20">
+        <v>0</v>
+      </c>
+      <c r="BT20">
+        <v>0</v>
+      </c>
+      <c r="BU20">
+        <v>0</v>
+      </c>
+      <c r="BV20">
+        <v>0</v>
+      </c>
+      <c r="BW20">
+        <v>0</v>
+      </c>
+      <c r="BX20">
+        <v>0</v>
+      </c>
+      <c r="BY20">
+        <v>0</v>
+      </c>
+      <c r="BZ20">
+        <v>0</v>
+      </c>
+      <c r="CA20">
+        <v>0</v>
+      </c>
+      <c r="CB20">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Latin names for pg. 179
</commit_message>
<xml_diff>
--- a/Lovejoy data table_Frequency of capture.xlsx
+++ b/Lovejoy data table_Frequency of capture.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
   <si>
     <t>Bird Species</t>
   </si>
@@ -62,15 +62,85 @@
   <si>
     <t>Chaetura spinicaudus</t>
   </si>
+  <si>
+    <t>Turdus albicollis</t>
+  </si>
+  <si>
+    <t>Coereba flaveola</t>
+  </si>
+  <si>
+    <t>Geothlypis aequinoctialis</t>
+  </si>
+  <si>
+    <t>Cyanocompsa cyanoides</t>
+  </si>
+  <si>
+    <t>Crypturellus cinereus</t>
+  </si>
+  <si>
+    <t>Leptodon cayanensis</t>
+  </si>
+  <si>
+    <t>Micrastur gilvicollis</t>
+  </si>
+  <si>
+    <t>Glaucis hirsuta</t>
+  </si>
+  <si>
+    <t>Trogon viridis</t>
+  </si>
+  <si>
+    <t>Ramphastos vitellinus</t>
+  </si>
+  <si>
+    <t>Notharchus macrorhynchos</t>
+  </si>
+  <si>
+    <t>Microcerculus marginatus</t>
+  </si>
+  <si>
+    <t>Synallaxis rutilans</t>
+  </si>
+  <si>
+    <t>Corythopis torquata</t>
+  </si>
+  <si>
+    <t>Thryothorus genibarbis</t>
+  </si>
+  <si>
+    <t>Turdus nudigenis</t>
+  </si>
+  <si>
+    <t>Cyanerpes caeruleus</t>
+  </si>
+  <si>
+    <t>Oryzoborus angolensis</t>
+  </si>
+  <si>
+    <t>Crypturellus soui</t>
+  </si>
+  <si>
+    <t>Harpagus bidentatus</t>
+  </si>
+  <si>
+    <t>Chaetura chapmani</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -96,8 +166,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -404,9 +475,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CB42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BK1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="BK35" sqref="BK35"/>
+      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5255,6 +5326,9 @@
       <c r="A21">
         <v>150</v>
       </c>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="C21">
         <v>129</v>
       </c>
@@ -5494,6 +5568,9 @@
       <c r="A22">
         <v>155</v>
       </c>
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
       <c r="C22">
         <v>0</v>
       </c>
@@ -5733,6 +5810,9 @@
       <c r="A23">
         <v>156</v>
       </c>
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
       <c r="C23">
         <v>6</v>
       </c>
@@ -5972,6 +6052,9 @@
       <c r="A24">
         <v>160</v>
       </c>
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
       <c r="C24">
         <v>226</v>
       </c>
@@ -6211,6 +6294,9 @@
       <c r="A25">
         <v>201</v>
       </c>
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
       <c r="C25">
         <v>1</v>
       </c>
@@ -6450,6 +6536,9 @@
       <c r="A26">
         <v>208</v>
       </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
       <c r="C26">
         <v>0</v>
       </c>
@@ -6689,6 +6778,9 @@
       <c r="A27">
         <v>209</v>
       </c>
+      <c r="B27" t="s">
+        <v>21</v>
+      </c>
       <c r="C27">
         <v>26</v>
       </c>
@@ -6928,6 +7020,9 @@
       <c r="A28">
         <v>225</v>
       </c>
+      <c r="B28" t="s">
+        <v>7</v>
+      </c>
       <c r="C28">
         <v>0</v>
       </c>
@@ -7167,6 +7262,9 @@
       <c r="A29">
         <v>231</v>
       </c>
+      <c r="B29" t="s">
+        <v>22</v>
+      </c>
       <c r="C29">
         <v>30</v>
       </c>
@@ -7406,6 +7504,9 @@
       <c r="A30">
         <v>232</v>
       </c>
+      <c r="B30" t="s">
+        <v>23</v>
+      </c>
       <c r="C30">
         <v>2</v>
       </c>
@@ -7645,6 +7746,9 @@
       <c r="A31">
         <v>236</v>
       </c>
+      <c r="B31" t="s">
+        <v>25</v>
+      </c>
       <c r="C31">
         <v>0</v>
       </c>
@@ -7884,6 +7988,9 @@
       <c r="A32">
         <v>237</v>
       </c>
+      <c r="B32" t="s">
+        <v>24</v>
+      </c>
       <c r="C32">
         <v>2</v>
       </c>
@@ -8123,6 +8230,9 @@
       <c r="A33">
         <v>238</v>
       </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
       <c r="C33">
         <v>0</v>
       </c>
@@ -8362,6 +8472,9 @@
       <c r="A34">
         <v>240</v>
       </c>
+      <c r="B34" t="s">
+        <v>27</v>
+      </c>
       <c r="C34">
         <v>47</v>
       </c>
@@ -8601,6 +8714,9 @@
       <c r="A35">
         <v>242</v>
       </c>
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
       <c r="C35">
         <v>33</v>
       </c>
@@ -8840,6 +8956,9 @@
       <c r="A36">
         <v>248</v>
       </c>
+      <c r="B36" t="s">
+        <v>29</v>
+      </c>
       <c r="C36">
         <v>7</v>
       </c>
@@ -9079,6 +9198,9 @@
       <c r="A37">
         <v>250</v>
       </c>
+      <c r="B37" t="s">
+        <v>30</v>
+      </c>
       <c r="C37">
         <v>4</v>
       </c>
@@ -9318,6 +9440,9 @@
       <c r="A38">
         <v>255</v>
       </c>
+      <c r="B38" t="s">
+        <v>31</v>
+      </c>
       <c r="C38">
         <v>10</v>
       </c>
@@ -9557,6 +9682,9 @@
       <c r="A39">
         <v>260</v>
       </c>
+      <c r="B39" t="s">
+        <v>32</v>
+      </c>
       <c r="C39">
         <v>6</v>
       </c>
@@ -9796,6 +9924,9 @@
       <c r="A40">
         <v>301</v>
       </c>
+      <c r="B40" t="s">
+        <v>33</v>
+      </c>
       <c r="C40">
         <v>2</v>
       </c>
@@ -10035,6 +10166,9 @@
       <c r="A41">
         <v>308</v>
       </c>
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
       <c r="C41">
         <v>3</v>
       </c>
@@ -10273,6 +10407,9 @@
     <row r="42" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>330</v>
+      </c>
+      <c r="B42" t="s">
+        <v>35</v>
       </c>
       <c r="C42">
         <v>0</v>

</xml_diff>

<commit_message>
added species ID # and frequency data for 11 rows (pg. 180); added Latin name for Pearly Breasted Cuckoo (pg. 179)
</commit_message>
<xml_diff>
--- a/Lovejoy data table_Frequency of capture.xlsx
+++ b/Lovejoy data table_Frequency of capture.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>Bird Species</t>
   </si>
@@ -124,6 +124,9 @@
   </si>
   <si>
     <t>Chaetura chapmani</t>
+  </si>
+  <si>
+    <t>Coccyzus euleri</t>
   </si>
 </sst>
 </file>
@@ -473,11 +476,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CB42"/>
+  <dimension ref="A1:CB64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AS60" sqref="AS60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7021,7 +7024,7 @@
         <v>225</v>
       </c>
       <c r="B28" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -10644,6 +10647,2720 @@
       </c>
       <c r="CB42">
         <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>331</v>
+      </c>
+      <c r="C43">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="44" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>336</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>0</v>
+      </c>
+      <c r="J44">
+        <v>0</v>
+      </c>
+      <c r="K44">
+        <v>0</v>
+      </c>
+      <c r="L44">
+        <v>0</v>
+      </c>
+      <c r="M44">
+        <v>0</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>0</v>
+      </c>
+      <c r="P44">
+        <v>0</v>
+      </c>
+      <c r="Q44">
+        <v>0</v>
+      </c>
+      <c r="R44">
+        <v>0</v>
+      </c>
+      <c r="S44">
+        <v>0</v>
+      </c>
+      <c r="T44">
+        <v>0</v>
+      </c>
+      <c r="U44">
+        <v>0</v>
+      </c>
+      <c r="V44">
+        <v>0</v>
+      </c>
+      <c r="W44">
+        <v>0</v>
+      </c>
+      <c r="X44">
+        <v>0</v>
+      </c>
+      <c r="Y44">
+        <v>0</v>
+      </c>
+      <c r="Z44">
+        <v>0</v>
+      </c>
+      <c r="AA44">
+        <v>0</v>
+      </c>
+      <c r="AB44">
+        <v>0</v>
+      </c>
+      <c r="AC44">
+        <v>0</v>
+      </c>
+      <c r="AD44">
+        <v>0</v>
+      </c>
+      <c r="AE44">
+        <v>0</v>
+      </c>
+      <c r="AF44">
+        <v>0</v>
+      </c>
+      <c r="AG44">
+        <v>0</v>
+      </c>
+      <c r="AH44">
+        <v>0</v>
+      </c>
+      <c r="AI44">
+        <v>0</v>
+      </c>
+      <c r="AJ44">
+        <v>0</v>
+      </c>
+      <c r="AK44">
+        <v>0</v>
+      </c>
+      <c r="AL44">
+        <v>0</v>
+      </c>
+      <c r="AM44">
+        <v>0</v>
+      </c>
+      <c r="AN44">
+        <v>0</v>
+      </c>
+      <c r="AO44">
+        <v>0</v>
+      </c>
+      <c r="AP44">
+        <v>0</v>
+      </c>
+      <c r="AQ44">
+        <v>0</v>
+      </c>
+      <c r="AR44">
+        <v>0</v>
+      </c>
+      <c r="AS44">
+        <v>0</v>
+      </c>
+      <c r="AT44">
+        <v>0</v>
+      </c>
+      <c r="AU44">
+        <v>0</v>
+      </c>
+      <c r="AV44">
+        <v>0</v>
+      </c>
+      <c r="AW44">
+        <v>0</v>
+      </c>
+      <c r="AX44">
+        <v>0</v>
+      </c>
+      <c r="AY44">
+        <v>0</v>
+      </c>
+      <c r="AZ44">
+        <v>0</v>
+      </c>
+      <c r="BA44">
+        <v>1</v>
+      </c>
+      <c r="BB44">
+        <v>0</v>
+      </c>
+      <c r="BC44">
+        <v>0</v>
+      </c>
+      <c r="BD44">
+        <v>0</v>
+      </c>
+      <c r="BE44">
+        <v>0</v>
+      </c>
+      <c r="BF44">
+        <v>0</v>
+      </c>
+      <c r="BG44">
+        <v>0</v>
+      </c>
+      <c r="BH44">
+        <v>0</v>
+      </c>
+      <c r="BI44">
+        <v>0</v>
+      </c>
+      <c r="BJ44">
+        <v>0</v>
+      </c>
+      <c r="BK44">
+        <v>0</v>
+      </c>
+      <c r="BL44">
+        <v>0</v>
+      </c>
+      <c r="BM44">
+        <v>0</v>
+      </c>
+      <c r="BN44">
+        <v>0</v>
+      </c>
+      <c r="BO44">
+        <v>0</v>
+      </c>
+      <c r="BP44">
+        <v>0</v>
+      </c>
+      <c r="BQ44">
+        <v>0</v>
+      </c>
+      <c r="BR44">
+        <v>0</v>
+      </c>
+      <c r="BS44">
+        <v>0</v>
+      </c>
+      <c r="BT44">
+        <v>0</v>
+      </c>
+      <c r="BU44">
+        <v>0</v>
+      </c>
+      <c r="BV44">
+        <v>0</v>
+      </c>
+      <c r="BW44">
+        <v>0</v>
+      </c>
+      <c r="BX44">
+        <v>0</v>
+      </c>
+      <c r="BY44">
+        <v>0</v>
+      </c>
+      <c r="BZ44">
+        <v>0</v>
+      </c>
+      <c r="CA44">
+        <v>0</v>
+      </c>
+      <c r="CB44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>337</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+      <c r="T45">
+        <v>0</v>
+      </c>
+      <c r="U45">
+        <v>0</v>
+      </c>
+      <c r="V45">
+        <v>0</v>
+      </c>
+      <c r="W45">
+        <v>0</v>
+      </c>
+      <c r="X45">
+        <v>0</v>
+      </c>
+      <c r="Y45">
+        <v>0</v>
+      </c>
+      <c r="Z45">
+        <v>0</v>
+      </c>
+      <c r="AA45">
+        <v>0</v>
+      </c>
+      <c r="AB45">
+        <v>0</v>
+      </c>
+      <c r="AC45">
+        <v>0</v>
+      </c>
+      <c r="AD45">
+        <v>0</v>
+      </c>
+      <c r="AE45">
+        <v>0</v>
+      </c>
+      <c r="AF45">
+        <v>0</v>
+      </c>
+      <c r="AG45">
+        <v>0</v>
+      </c>
+      <c r="AH45">
+        <v>0</v>
+      </c>
+      <c r="AI45">
+        <v>0</v>
+      </c>
+      <c r="AJ45">
+        <v>0</v>
+      </c>
+      <c r="AK45">
+        <v>0</v>
+      </c>
+      <c r="AL45">
+        <v>0</v>
+      </c>
+      <c r="AM45">
+        <v>0</v>
+      </c>
+      <c r="AN45">
+        <v>0</v>
+      </c>
+      <c r="AO45">
+        <v>0</v>
+      </c>
+      <c r="AP45">
+        <v>0</v>
+      </c>
+      <c r="AQ45">
+        <v>0</v>
+      </c>
+      <c r="AR45">
+        <v>0</v>
+      </c>
+      <c r="AS45">
+        <v>0</v>
+      </c>
+      <c r="AT45">
+        <v>0</v>
+      </c>
+      <c r="AU45">
+        <v>0</v>
+      </c>
+      <c r="AV45">
+        <v>0</v>
+      </c>
+      <c r="AW45">
+        <v>0</v>
+      </c>
+      <c r="AX45">
+        <v>0</v>
+      </c>
+      <c r="AY45">
+        <v>0</v>
+      </c>
+      <c r="AZ45">
+        <v>0</v>
+      </c>
+      <c r="BA45">
+        <v>0</v>
+      </c>
+      <c r="BB45">
+        <v>0</v>
+      </c>
+      <c r="BC45">
+        <v>0</v>
+      </c>
+      <c r="BD45">
+        <v>0</v>
+      </c>
+      <c r="BE45">
+        <v>0</v>
+      </c>
+      <c r="BF45">
+        <v>0</v>
+      </c>
+      <c r="BG45">
+        <v>0</v>
+      </c>
+      <c r="BH45">
+        <v>0</v>
+      </c>
+      <c r="BI45">
+        <v>0</v>
+      </c>
+      <c r="BJ45">
+        <v>0</v>
+      </c>
+      <c r="BK45">
+        <v>0</v>
+      </c>
+      <c r="BL45">
+        <v>0</v>
+      </c>
+      <c r="BM45">
+        <v>0</v>
+      </c>
+      <c r="BN45">
+        <v>0</v>
+      </c>
+      <c r="BO45">
+        <v>0</v>
+      </c>
+      <c r="BP45">
+        <v>0</v>
+      </c>
+      <c r="BQ45">
+        <v>0</v>
+      </c>
+      <c r="BR45">
+        <v>0</v>
+      </c>
+      <c r="BS45">
+        <v>0</v>
+      </c>
+      <c r="BT45">
+        <v>0</v>
+      </c>
+      <c r="BU45">
+        <v>0</v>
+      </c>
+      <c r="BV45">
+        <v>0</v>
+      </c>
+      <c r="BW45">
+        <v>0</v>
+      </c>
+      <c r="BX45">
+        <v>0</v>
+      </c>
+      <c r="BY45">
+        <v>0</v>
+      </c>
+      <c r="BZ45">
+        <v>0</v>
+      </c>
+      <c r="CA45">
+        <v>0</v>
+      </c>
+      <c r="CB45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>343</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>0</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>0</v>
+      </c>
+      <c r="T46">
+        <v>0</v>
+      </c>
+      <c r="U46">
+        <v>0</v>
+      </c>
+      <c r="V46">
+        <v>0</v>
+      </c>
+      <c r="W46">
+        <v>0</v>
+      </c>
+      <c r="X46">
+        <v>0</v>
+      </c>
+      <c r="Y46">
+        <v>0</v>
+      </c>
+      <c r="Z46">
+        <v>0</v>
+      </c>
+      <c r="AA46">
+        <v>0</v>
+      </c>
+      <c r="AB46">
+        <v>0</v>
+      </c>
+      <c r="AC46">
+        <v>0</v>
+      </c>
+      <c r="AD46">
+        <v>0</v>
+      </c>
+      <c r="AE46">
+        <v>0</v>
+      </c>
+      <c r="AF46">
+        <v>0</v>
+      </c>
+      <c r="AG46">
+        <v>0</v>
+      </c>
+      <c r="AH46">
+        <v>0</v>
+      </c>
+      <c r="AI46">
+        <v>0</v>
+      </c>
+      <c r="AJ46">
+        <v>0</v>
+      </c>
+      <c r="AK46">
+        <v>0</v>
+      </c>
+      <c r="AL46">
+        <v>0</v>
+      </c>
+      <c r="AM46">
+        <v>0</v>
+      </c>
+      <c r="AN46">
+        <v>0</v>
+      </c>
+      <c r="AO46">
+        <v>0</v>
+      </c>
+      <c r="AP46">
+        <v>0</v>
+      </c>
+      <c r="AQ46">
+        <v>0</v>
+      </c>
+      <c r="AR46">
+        <v>0</v>
+      </c>
+      <c r="AS46">
+        <v>0</v>
+      </c>
+      <c r="AT46">
+        <v>0</v>
+      </c>
+      <c r="AU46">
+        <v>0</v>
+      </c>
+      <c r="AV46">
+        <v>0</v>
+      </c>
+      <c r="AW46">
+        <v>0</v>
+      </c>
+      <c r="AX46">
+        <v>0</v>
+      </c>
+      <c r="AY46">
+        <v>0</v>
+      </c>
+      <c r="AZ46">
+        <v>0</v>
+      </c>
+      <c r="BA46">
+        <v>0</v>
+      </c>
+      <c r="BB46">
+        <v>0</v>
+      </c>
+      <c r="BC46">
+        <v>0</v>
+      </c>
+      <c r="BD46">
+        <v>0</v>
+      </c>
+      <c r="BE46">
+        <v>0</v>
+      </c>
+      <c r="BF46">
+        <v>0</v>
+      </c>
+      <c r="BG46">
+        <v>0</v>
+      </c>
+      <c r="BH46">
+        <v>0</v>
+      </c>
+      <c r="BI46">
+        <v>0</v>
+      </c>
+      <c r="BJ46">
+        <v>0</v>
+      </c>
+      <c r="BK46">
+        <v>0</v>
+      </c>
+      <c r="BL46">
+        <v>0</v>
+      </c>
+      <c r="BM46">
+        <v>0</v>
+      </c>
+      <c r="BN46">
+        <v>0</v>
+      </c>
+      <c r="BO46">
+        <v>0</v>
+      </c>
+      <c r="BP46">
+        <v>0</v>
+      </c>
+      <c r="BQ46">
+        <v>0</v>
+      </c>
+      <c r="BR46">
+        <v>0</v>
+      </c>
+      <c r="BS46">
+        <v>0</v>
+      </c>
+      <c r="BT46">
+        <v>0</v>
+      </c>
+      <c r="BU46">
+        <v>0</v>
+      </c>
+      <c r="BV46">
+        <v>0</v>
+      </c>
+      <c r="BW46">
+        <v>0</v>
+      </c>
+      <c r="BX46">
+        <v>0</v>
+      </c>
+      <c r="BY46">
+        <v>0</v>
+      </c>
+      <c r="BZ46">
+        <v>0</v>
+      </c>
+      <c r="CA46">
+        <v>0</v>
+      </c>
+      <c r="CB46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>344</v>
+      </c>
+      <c r="C47">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>350</v>
+      </c>
+      <c r="C48">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>351</v>
+      </c>
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>1</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+      <c r="I49">
+        <v>1</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>0</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>0</v>
+      </c>
+      <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="S49">
+        <v>0</v>
+      </c>
+      <c r="T49">
+        <v>0</v>
+      </c>
+      <c r="U49">
+        <v>0</v>
+      </c>
+      <c r="V49">
+        <v>0</v>
+      </c>
+      <c r="W49">
+        <v>0</v>
+      </c>
+      <c r="X49">
+        <v>0</v>
+      </c>
+      <c r="Y49">
+        <v>0</v>
+      </c>
+      <c r="Z49">
+        <v>0</v>
+      </c>
+      <c r="AA49">
+        <v>0</v>
+      </c>
+      <c r="AB49">
+        <v>0</v>
+      </c>
+      <c r="AC49">
+        <v>0</v>
+      </c>
+      <c r="AD49">
+        <v>0</v>
+      </c>
+      <c r="AE49">
+        <v>0</v>
+      </c>
+      <c r="AF49">
+        <v>0</v>
+      </c>
+      <c r="AG49">
+        <v>0</v>
+      </c>
+      <c r="AH49">
+        <v>0</v>
+      </c>
+      <c r="AI49">
+        <v>0</v>
+      </c>
+      <c r="AJ49">
+        <v>0</v>
+      </c>
+      <c r="AK49">
+        <v>0</v>
+      </c>
+      <c r="AL49">
+        <v>0</v>
+      </c>
+      <c r="AM49">
+        <v>0</v>
+      </c>
+      <c r="AN49">
+        <v>0</v>
+      </c>
+      <c r="AO49">
+        <v>0</v>
+      </c>
+      <c r="AP49">
+        <v>0</v>
+      </c>
+      <c r="AQ49">
+        <v>0</v>
+      </c>
+      <c r="AR49">
+        <v>0</v>
+      </c>
+      <c r="AS49">
+        <v>2</v>
+      </c>
+      <c r="AT49">
+        <v>0</v>
+      </c>
+      <c r="AU49">
+        <v>0</v>
+      </c>
+      <c r="AV49">
+        <v>0</v>
+      </c>
+      <c r="AW49">
+        <v>0</v>
+      </c>
+      <c r="AX49">
+        <v>0</v>
+      </c>
+      <c r="AY49">
+        <v>0</v>
+      </c>
+      <c r="AZ49">
+        <v>0</v>
+      </c>
+      <c r="BA49">
+        <v>0</v>
+      </c>
+      <c r="BB49">
+        <v>0</v>
+      </c>
+      <c r="BC49">
+        <v>3</v>
+      </c>
+      <c r="BD49">
+        <v>0</v>
+      </c>
+      <c r="BE49">
+        <v>0</v>
+      </c>
+      <c r="BF49">
+        <v>0</v>
+      </c>
+      <c r="BG49">
+        <v>0</v>
+      </c>
+      <c r="BH49">
+        <v>0</v>
+      </c>
+      <c r="BI49">
+        <v>0</v>
+      </c>
+      <c r="BJ49">
+        <v>0</v>
+      </c>
+      <c r="BK49">
+        <v>0</v>
+      </c>
+      <c r="BL49">
+        <v>0</v>
+      </c>
+      <c r="BM49">
+        <v>0</v>
+      </c>
+      <c r="BN49">
+        <v>0</v>
+      </c>
+      <c r="BO49">
+        <v>0</v>
+      </c>
+      <c r="BP49">
+        <v>0</v>
+      </c>
+      <c r="BQ49">
+        <v>0</v>
+      </c>
+      <c r="BR49">
+        <v>0</v>
+      </c>
+      <c r="BS49">
+        <v>0</v>
+      </c>
+      <c r="BT49">
+        <v>0</v>
+      </c>
+      <c r="BU49">
+        <v>0</v>
+      </c>
+      <c r="BV49">
+        <v>0</v>
+      </c>
+      <c r="BW49">
+        <v>0</v>
+      </c>
+      <c r="BX49">
+        <v>0</v>
+      </c>
+      <c r="BY49">
+        <v>0</v>
+      </c>
+      <c r="BZ49">
+        <v>0</v>
+      </c>
+      <c r="CA49">
+        <v>0</v>
+      </c>
+      <c r="CB49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>355</v>
+      </c>
+      <c r="C50">
+        <v>2</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>0</v>
+      </c>
+      <c r="J50">
+        <v>1</v>
+      </c>
+      <c r="K50">
+        <v>0</v>
+      </c>
+      <c r="L50">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>0</v>
+      </c>
+      <c r="P50">
+        <v>0</v>
+      </c>
+      <c r="Q50">
+        <v>0</v>
+      </c>
+      <c r="R50">
+        <v>0</v>
+      </c>
+      <c r="S50">
+        <v>0</v>
+      </c>
+      <c r="T50">
+        <v>0</v>
+      </c>
+      <c r="U50">
+        <v>0</v>
+      </c>
+      <c r="V50">
+        <v>0</v>
+      </c>
+      <c r="W50">
+        <v>0</v>
+      </c>
+      <c r="X50">
+        <v>0</v>
+      </c>
+      <c r="Y50">
+        <v>0</v>
+      </c>
+      <c r="Z50">
+        <v>0</v>
+      </c>
+      <c r="AA50">
+        <v>0</v>
+      </c>
+      <c r="AB50">
+        <v>0</v>
+      </c>
+      <c r="AC50">
+        <v>0</v>
+      </c>
+      <c r="AD50">
+        <v>0</v>
+      </c>
+      <c r="AE50">
+        <v>0</v>
+      </c>
+      <c r="AF50">
+        <v>0</v>
+      </c>
+      <c r="AG50">
+        <v>0</v>
+      </c>
+      <c r="AH50">
+        <v>0</v>
+      </c>
+      <c r="AI50">
+        <v>0</v>
+      </c>
+      <c r="AJ50">
+        <v>0</v>
+      </c>
+      <c r="AK50">
+        <v>0</v>
+      </c>
+      <c r="AL50">
+        <v>0</v>
+      </c>
+      <c r="AM50">
+        <v>0</v>
+      </c>
+      <c r="AN50">
+        <v>0</v>
+      </c>
+      <c r="AO50">
+        <v>0</v>
+      </c>
+      <c r="AP50">
+        <v>0</v>
+      </c>
+      <c r="AQ50">
+        <v>0</v>
+      </c>
+      <c r="AR50">
+        <v>0</v>
+      </c>
+      <c r="AS50">
+        <v>0</v>
+      </c>
+      <c r="AT50">
+        <v>0</v>
+      </c>
+      <c r="AU50">
+        <v>0</v>
+      </c>
+      <c r="AV50">
+        <v>0</v>
+      </c>
+      <c r="AW50">
+        <v>0</v>
+      </c>
+      <c r="AX50">
+        <v>0</v>
+      </c>
+      <c r="AY50">
+        <v>0</v>
+      </c>
+      <c r="AZ50">
+        <v>0</v>
+      </c>
+      <c r="BA50">
+        <v>1</v>
+      </c>
+      <c r="BB50">
+        <v>0</v>
+      </c>
+      <c r="BC50">
+        <v>0</v>
+      </c>
+      <c r="BD50">
+        <v>0</v>
+      </c>
+      <c r="BE50">
+        <v>0</v>
+      </c>
+      <c r="BF50">
+        <v>0</v>
+      </c>
+      <c r="BG50">
+        <v>0</v>
+      </c>
+      <c r="BH50">
+        <v>0</v>
+      </c>
+      <c r="BI50">
+        <v>0</v>
+      </c>
+      <c r="BJ50">
+        <v>0</v>
+      </c>
+      <c r="BK50">
+        <v>0</v>
+      </c>
+      <c r="BL50">
+        <v>0</v>
+      </c>
+      <c r="BM50">
+        <v>0</v>
+      </c>
+      <c r="BN50">
+        <v>0</v>
+      </c>
+      <c r="BO50">
+        <v>0</v>
+      </c>
+      <c r="BP50">
+        <v>0</v>
+      </c>
+      <c r="BQ50">
+        <v>0</v>
+      </c>
+      <c r="BR50">
+        <v>0</v>
+      </c>
+      <c r="BS50">
+        <v>0</v>
+      </c>
+      <c r="BT50">
+        <v>0</v>
+      </c>
+      <c r="BU50">
+        <v>0</v>
+      </c>
+      <c r="BV50">
+        <v>0</v>
+      </c>
+      <c r="BW50">
+        <v>0</v>
+      </c>
+      <c r="BX50">
+        <v>0</v>
+      </c>
+      <c r="BY50">
+        <v>0</v>
+      </c>
+      <c r="BZ50">
+        <v>0</v>
+      </c>
+      <c r="CA50">
+        <v>0</v>
+      </c>
+      <c r="CB50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>356</v>
+      </c>
+      <c r="C51">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="52" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>359</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>0</v>
+      </c>
+      <c r="L52">
+        <v>0</v>
+      </c>
+      <c r="M52">
+        <v>0</v>
+      </c>
+      <c r="N52">
+        <v>0</v>
+      </c>
+      <c r="O52">
+        <v>0</v>
+      </c>
+      <c r="P52">
+        <v>0</v>
+      </c>
+      <c r="Q52">
+        <v>0</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+      <c r="S52">
+        <v>0</v>
+      </c>
+      <c r="T52">
+        <v>0</v>
+      </c>
+      <c r="U52">
+        <v>0</v>
+      </c>
+      <c r="V52">
+        <v>0</v>
+      </c>
+      <c r="W52">
+        <v>0</v>
+      </c>
+      <c r="X52">
+        <v>0</v>
+      </c>
+      <c r="Y52">
+        <v>0</v>
+      </c>
+      <c r="Z52">
+        <v>0</v>
+      </c>
+      <c r="AA52">
+        <v>0</v>
+      </c>
+      <c r="AB52">
+        <v>0</v>
+      </c>
+      <c r="AC52">
+        <v>0</v>
+      </c>
+      <c r="AD52">
+        <v>0</v>
+      </c>
+      <c r="AE52">
+        <v>0</v>
+      </c>
+      <c r="AF52">
+        <v>0</v>
+      </c>
+      <c r="AG52">
+        <v>0</v>
+      </c>
+      <c r="AH52">
+        <v>0</v>
+      </c>
+      <c r="AI52">
+        <v>0</v>
+      </c>
+      <c r="AJ52">
+        <v>0</v>
+      </c>
+      <c r="AK52">
+        <v>0</v>
+      </c>
+      <c r="AL52">
+        <v>0</v>
+      </c>
+      <c r="AM52">
+        <v>0</v>
+      </c>
+      <c r="AN52">
+        <v>0</v>
+      </c>
+      <c r="AO52">
+        <v>0</v>
+      </c>
+      <c r="AP52">
+        <v>0</v>
+      </c>
+      <c r="AQ52">
+        <v>0</v>
+      </c>
+      <c r="AR52">
+        <v>0</v>
+      </c>
+      <c r="AS52">
+        <v>0</v>
+      </c>
+      <c r="AT52">
+        <v>0</v>
+      </c>
+      <c r="AU52">
+        <v>0</v>
+      </c>
+      <c r="AV52">
+        <v>0</v>
+      </c>
+      <c r="AW52">
+        <v>0</v>
+      </c>
+      <c r="AX52">
+        <v>0</v>
+      </c>
+      <c r="AY52">
+        <v>0</v>
+      </c>
+      <c r="AZ52">
+        <v>0</v>
+      </c>
+      <c r="BA52">
+        <v>0</v>
+      </c>
+      <c r="BB52">
+        <v>0</v>
+      </c>
+      <c r="BC52">
+        <v>0</v>
+      </c>
+      <c r="BD52">
+        <v>0</v>
+      </c>
+      <c r="BE52">
+        <v>0</v>
+      </c>
+      <c r="BF52">
+        <v>0</v>
+      </c>
+      <c r="BG52">
+        <v>0</v>
+      </c>
+      <c r="BH52">
+        <v>0</v>
+      </c>
+      <c r="BI52">
+        <v>0</v>
+      </c>
+      <c r="BJ52">
+        <v>0</v>
+      </c>
+      <c r="BK52">
+        <v>0</v>
+      </c>
+      <c r="BL52">
+        <v>0</v>
+      </c>
+      <c r="BM52">
+        <v>0</v>
+      </c>
+      <c r="BN52">
+        <v>0</v>
+      </c>
+      <c r="BO52">
+        <v>0</v>
+      </c>
+      <c r="BP52">
+        <v>0</v>
+      </c>
+      <c r="BQ52">
+        <v>0</v>
+      </c>
+      <c r="BR52">
+        <v>0</v>
+      </c>
+      <c r="BS52">
+        <v>0</v>
+      </c>
+      <c r="BT52">
+        <v>0</v>
+      </c>
+      <c r="BU52">
+        <v>0</v>
+      </c>
+      <c r="BV52">
+        <v>0</v>
+      </c>
+      <c r="BW52">
+        <v>0</v>
+      </c>
+      <c r="BX52">
+        <v>0</v>
+      </c>
+      <c r="BY52">
+        <v>0</v>
+      </c>
+      <c r="BZ52">
+        <v>0</v>
+      </c>
+      <c r="CA52">
+        <v>0</v>
+      </c>
+      <c r="CB52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>425</v>
+      </c>
+      <c r="C53">
+        <v>6</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>0</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+      <c r="N53">
+        <v>0</v>
+      </c>
+      <c r="O53">
+        <v>0</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="Q53">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>0</v>
+      </c>
+      <c r="S53">
+        <v>0</v>
+      </c>
+      <c r="T53">
+        <v>0</v>
+      </c>
+      <c r="U53">
+        <v>0</v>
+      </c>
+      <c r="V53">
+        <v>0</v>
+      </c>
+      <c r="W53">
+        <v>0</v>
+      </c>
+      <c r="X53">
+        <v>0</v>
+      </c>
+      <c r="Y53">
+        <v>0</v>
+      </c>
+      <c r="Z53">
+        <v>0</v>
+      </c>
+      <c r="AA53">
+        <v>0</v>
+      </c>
+      <c r="AB53">
+        <v>0</v>
+      </c>
+      <c r="AC53">
+        <v>0</v>
+      </c>
+      <c r="AD53">
+        <v>0</v>
+      </c>
+      <c r="AE53">
+        <v>0</v>
+      </c>
+      <c r="AF53">
+        <v>0</v>
+      </c>
+      <c r="AG53">
+        <v>0</v>
+      </c>
+      <c r="AH53">
+        <v>0</v>
+      </c>
+      <c r="AI53">
+        <v>0</v>
+      </c>
+      <c r="AJ53">
+        <v>0</v>
+      </c>
+      <c r="AK53">
+        <v>0</v>
+      </c>
+      <c r="AL53">
+        <v>0</v>
+      </c>
+      <c r="AM53">
+        <v>0</v>
+      </c>
+      <c r="AN53">
+        <v>0</v>
+      </c>
+      <c r="AO53">
+        <v>0</v>
+      </c>
+      <c r="AP53">
+        <v>0</v>
+      </c>
+      <c r="AQ53">
+        <v>0</v>
+      </c>
+      <c r="AR53">
+        <v>0</v>
+      </c>
+      <c r="AS53">
+        <v>0</v>
+      </c>
+      <c r="AT53">
+        <v>0</v>
+      </c>
+      <c r="AU53">
+        <v>0</v>
+      </c>
+      <c r="AV53">
+        <v>0</v>
+      </c>
+      <c r="AW53">
+        <v>0</v>
+      </c>
+      <c r="AX53">
+        <v>0</v>
+      </c>
+      <c r="AY53">
+        <v>0</v>
+      </c>
+      <c r="AZ53">
+        <v>0</v>
+      </c>
+      <c r="BA53">
+        <v>0</v>
+      </c>
+      <c r="BB53">
+        <v>0</v>
+      </c>
+      <c r="BC53">
+        <v>0</v>
+      </c>
+      <c r="BD53">
+        <v>0</v>
+      </c>
+      <c r="BE53">
+        <v>0</v>
+      </c>
+      <c r="BF53">
+        <v>0</v>
+      </c>
+      <c r="BG53">
+        <v>0</v>
+      </c>
+      <c r="BH53">
+        <v>0</v>
+      </c>
+      <c r="BI53">
+        <v>0</v>
+      </c>
+      <c r="BJ53">
+        <v>0</v>
+      </c>
+      <c r="BK53">
+        <v>0</v>
+      </c>
+      <c r="BL53">
+        <v>0</v>
+      </c>
+      <c r="BM53">
+        <v>0</v>
+      </c>
+      <c r="BN53">
+        <v>0</v>
+      </c>
+      <c r="BO53">
+        <v>0</v>
+      </c>
+      <c r="BP53">
+        <v>0</v>
+      </c>
+      <c r="BQ53">
+        <v>0</v>
+      </c>
+      <c r="BR53">
+        <v>1</v>
+      </c>
+      <c r="BS53">
+        <v>0</v>
+      </c>
+      <c r="BT53">
+        <v>1</v>
+      </c>
+      <c r="BU53">
+        <v>0</v>
+      </c>
+      <c r="BV53">
+        <v>0</v>
+      </c>
+      <c r="BW53">
+        <v>0</v>
+      </c>
+      <c r="BX53">
+        <v>0</v>
+      </c>
+      <c r="BY53">
+        <v>0</v>
+      </c>
+      <c r="BZ53">
+        <v>3</v>
+      </c>
+      <c r="CA53">
+        <v>1</v>
+      </c>
+      <c r="CB53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>429</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>1</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+      <c r="I54">
+        <v>0</v>
+      </c>
+      <c r="J54">
+        <v>0</v>
+      </c>
+      <c r="K54">
+        <v>0</v>
+      </c>
+      <c r="L54">
+        <v>0</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+      <c r="N54">
+        <v>0</v>
+      </c>
+      <c r="O54">
+        <v>0</v>
+      </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
+      <c r="Q54">
+        <v>0</v>
+      </c>
+      <c r="R54">
+        <v>0</v>
+      </c>
+      <c r="S54">
+        <v>0</v>
+      </c>
+      <c r="T54">
+        <v>0</v>
+      </c>
+      <c r="U54">
+        <v>0</v>
+      </c>
+      <c r="V54">
+        <v>0</v>
+      </c>
+      <c r="W54">
+        <v>0</v>
+      </c>
+      <c r="X54">
+        <v>0</v>
+      </c>
+      <c r="Y54">
+        <v>0</v>
+      </c>
+      <c r="Z54">
+        <v>0</v>
+      </c>
+      <c r="AA54">
+        <v>0</v>
+      </c>
+      <c r="AB54">
+        <v>0</v>
+      </c>
+      <c r="AC54">
+        <v>0</v>
+      </c>
+      <c r="AD54">
+        <v>0</v>
+      </c>
+      <c r="AE54">
+        <v>0</v>
+      </c>
+      <c r="AF54">
+        <v>0</v>
+      </c>
+      <c r="AG54">
+        <v>0</v>
+      </c>
+      <c r="AH54">
+        <v>0</v>
+      </c>
+      <c r="AI54">
+        <v>0</v>
+      </c>
+      <c r="AJ54">
+        <v>0</v>
+      </c>
+      <c r="AK54">
+        <v>0</v>
+      </c>
+      <c r="AL54">
+        <v>0</v>
+      </c>
+      <c r="AM54">
+        <v>0</v>
+      </c>
+      <c r="AN54">
+        <v>0</v>
+      </c>
+      <c r="AO54">
+        <v>0</v>
+      </c>
+      <c r="AP54">
+        <v>0</v>
+      </c>
+      <c r="AQ54">
+        <v>0</v>
+      </c>
+      <c r="AR54">
+        <v>0</v>
+      </c>
+      <c r="AS54">
+        <v>0</v>
+      </c>
+      <c r="AT54">
+        <v>0</v>
+      </c>
+      <c r="AU54">
+        <v>0</v>
+      </c>
+      <c r="AV54">
+        <v>0</v>
+      </c>
+      <c r="AW54">
+        <v>0</v>
+      </c>
+      <c r="AX54">
+        <v>0</v>
+      </c>
+      <c r="AY54">
+        <v>0</v>
+      </c>
+      <c r="AZ54">
+        <v>0</v>
+      </c>
+      <c r="BA54">
+        <v>0</v>
+      </c>
+      <c r="BB54">
+        <v>0</v>
+      </c>
+      <c r="BC54">
+        <v>0</v>
+      </c>
+      <c r="BD54">
+        <v>0</v>
+      </c>
+      <c r="BE54">
+        <v>0</v>
+      </c>
+      <c r="BF54">
+        <v>0</v>
+      </c>
+      <c r="BG54">
+        <v>0</v>
+      </c>
+      <c r="BH54">
+        <v>0</v>
+      </c>
+      <c r="BI54">
+        <v>0</v>
+      </c>
+      <c r="BJ54">
+        <v>0</v>
+      </c>
+      <c r="BK54">
+        <v>0</v>
+      </c>
+      <c r="BL54">
+        <v>0</v>
+      </c>
+      <c r="BM54">
+        <v>0</v>
+      </c>
+      <c r="BN54">
+        <v>0</v>
+      </c>
+      <c r="BO54">
+        <v>0</v>
+      </c>
+      <c r="BP54">
+        <v>0</v>
+      </c>
+      <c r="BQ54">
+        <v>0</v>
+      </c>
+      <c r="BR54">
+        <v>0</v>
+      </c>
+      <c r="BS54">
+        <v>0</v>
+      </c>
+      <c r="BT54">
+        <v>0</v>
+      </c>
+      <c r="BU54">
+        <v>0</v>
+      </c>
+      <c r="BV54">
+        <v>0</v>
+      </c>
+      <c r="BW54">
+        <v>0</v>
+      </c>
+      <c r="BX54">
+        <v>0</v>
+      </c>
+      <c r="BY54">
+        <v>0</v>
+      </c>
+      <c r="BZ54">
+        <v>0</v>
+      </c>
+      <c r="CA54">
+        <v>0</v>
+      </c>
+      <c r="CB54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>431</v>
+      </c>
+      <c r="C55">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>432</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+      <c r="I56">
+        <v>0</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>0</v>
+      </c>
+      <c r="L56">
+        <v>0</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+      <c r="N56">
+        <v>0</v>
+      </c>
+      <c r="O56">
+        <v>0</v>
+      </c>
+      <c r="P56">
+        <v>0</v>
+      </c>
+      <c r="Q56">
+        <v>0</v>
+      </c>
+      <c r="R56">
+        <v>0</v>
+      </c>
+      <c r="S56">
+        <v>0</v>
+      </c>
+      <c r="T56">
+        <v>0</v>
+      </c>
+      <c r="U56">
+        <v>0</v>
+      </c>
+      <c r="V56">
+        <v>0</v>
+      </c>
+      <c r="W56">
+        <v>0</v>
+      </c>
+      <c r="X56">
+        <v>0</v>
+      </c>
+      <c r="Y56">
+        <v>0</v>
+      </c>
+      <c r="Z56">
+        <v>0</v>
+      </c>
+      <c r="AA56">
+        <v>0</v>
+      </c>
+      <c r="AB56">
+        <v>0</v>
+      </c>
+      <c r="AC56">
+        <v>0</v>
+      </c>
+      <c r="AD56">
+        <v>0</v>
+      </c>
+      <c r="AE56">
+        <v>0</v>
+      </c>
+      <c r="AF56">
+        <v>0</v>
+      </c>
+      <c r="AG56">
+        <v>0</v>
+      </c>
+      <c r="AH56">
+        <v>0</v>
+      </c>
+      <c r="AI56">
+        <v>0</v>
+      </c>
+      <c r="AJ56">
+        <v>0</v>
+      </c>
+      <c r="AK56">
+        <v>0</v>
+      </c>
+      <c r="AL56">
+        <v>0</v>
+      </c>
+      <c r="AM56">
+        <v>0</v>
+      </c>
+      <c r="AN56">
+        <v>0</v>
+      </c>
+      <c r="AO56">
+        <v>0</v>
+      </c>
+      <c r="AP56">
+        <v>0</v>
+      </c>
+      <c r="AQ56">
+        <v>0</v>
+      </c>
+      <c r="AR56">
+        <v>0</v>
+      </c>
+      <c r="AS56">
+        <v>0</v>
+      </c>
+      <c r="AT56">
+        <v>0</v>
+      </c>
+      <c r="AU56">
+        <v>0</v>
+      </c>
+      <c r="AV56">
+        <v>0</v>
+      </c>
+      <c r="AW56">
+        <v>0</v>
+      </c>
+      <c r="AX56">
+        <v>0</v>
+      </c>
+      <c r="AY56">
+        <v>0</v>
+      </c>
+      <c r="AZ56">
+        <v>0</v>
+      </c>
+      <c r="BA56">
+        <v>0</v>
+      </c>
+      <c r="BB56">
+        <v>0</v>
+      </c>
+      <c r="BC56">
+        <v>0</v>
+      </c>
+      <c r="BD56">
+        <v>0</v>
+      </c>
+      <c r="BE56">
+        <v>0</v>
+      </c>
+      <c r="BF56">
+        <v>0</v>
+      </c>
+      <c r="BG56">
+        <v>0</v>
+      </c>
+      <c r="BH56">
+        <v>0</v>
+      </c>
+      <c r="BI56">
+        <v>0</v>
+      </c>
+      <c r="BJ56">
+        <v>0</v>
+      </c>
+      <c r="BK56">
+        <v>0</v>
+      </c>
+      <c r="BL56">
+        <v>0</v>
+      </c>
+      <c r="BM56">
+        <v>0</v>
+      </c>
+      <c r="BN56">
+        <v>0</v>
+      </c>
+      <c r="BO56">
+        <v>0</v>
+      </c>
+      <c r="BP56">
+        <v>0</v>
+      </c>
+      <c r="BQ56">
+        <v>0</v>
+      </c>
+      <c r="BR56">
+        <v>0</v>
+      </c>
+      <c r="BS56">
+        <v>0</v>
+      </c>
+      <c r="BT56">
+        <v>0</v>
+      </c>
+      <c r="BU56">
+        <v>0</v>
+      </c>
+      <c r="BV56">
+        <v>0</v>
+      </c>
+      <c r="BW56">
+        <v>0</v>
+      </c>
+      <c r="BX56">
+        <v>0</v>
+      </c>
+      <c r="BY56">
+        <v>0</v>
+      </c>
+      <c r="BZ56">
+        <v>0</v>
+      </c>
+      <c r="CA56">
+        <v>1</v>
+      </c>
+      <c r="CB56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>433</v>
+      </c>
+      <c r="C57">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>437</v>
+      </c>
+      <c r="C58">
+        <v>7</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>4</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>1</v>
+      </c>
+      <c r="K58">
+        <v>0</v>
+      </c>
+      <c r="L58">
+        <v>0</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+      <c r="N58">
+        <v>0</v>
+      </c>
+      <c r="O58">
+        <v>0</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+      <c r="Q58">
+        <v>0</v>
+      </c>
+      <c r="R58">
+        <v>0</v>
+      </c>
+      <c r="S58">
+        <v>0</v>
+      </c>
+      <c r="T58">
+        <v>0</v>
+      </c>
+      <c r="U58">
+        <v>0</v>
+      </c>
+      <c r="V58">
+        <v>0</v>
+      </c>
+      <c r="W58">
+        <v>0</v>
+      </c>
+      <c r="X58">
+        <v>0</v>
+      </c>
+      <c r="Y58">
+        <v>0</v>
+      </c>
+      <c r="Z58">
+        <v>0</v>
+      </c>
+      <c r="AA58">
+        <v>0</v>
+      </c>
+      <c r="AB58">
+        <v>0</v>
+      </c>
+      <c r="AC58">
+        <v>0</v>
+      </c>
+      <c r="AD58">
+        <v>0</v>
+      </c>
+      <c r="AE58">
+        <v>0</v>
+      </c>
+      <c r="AF58">
+        <v>0</v>
+      </c>
+      <c r="AG58">
+        <v>0</v>
+      </c>
+      <c r="AH58">
+        <v>0</v>
+      </c>
+      <c r="AI58">
+        <v>0</v>
+      </c>
+      <c r="AJ58">
+        <v>0</v>
+      </c>
+      <c r="AK58">
+        <v>0</v>
+      </c>
+      <c r="AL58">
+        <v>0</v>
+      </c>
+      <c r="AM58">
+        <v>0</v>
+      </c>
+      <c r="AN58">
+        <v>0</v>
+      </c>
+      <c r="AO58">
+        <v>0</v>
+      </c>
+      <c r="AP58">
+        <v>0</v>
+      </c>
+      <c r="AQ58">
+        <v>0</v>
+      </c>
+      <c r="AR58">
+        <v>0</v>
+      </c>
+      <c r="AS58">
+        <v>2</v>
+      </c>
+      <c r="AT58">
+        <v>0</v>
+      </c>
+      <c r="AU58">
+        <v>0</v>
+      </c>
+      <c r="AV58">
+        <v>0</v>
+      </c>
+      <c r="AW58">
+        <v>0</v>
+      </c>
+      <c r="AX58">
+        <v>0</v>
+      </c>
+      <c r="AY58">
+        <v>0</v>
+      </c>
+      <c r="AZ58">
+        <v>0</v>
+      </c>
+      <c r="BA58">
+        <v>0</v>
+      </c>
+      <c r="BB58">
+        <v>0</v>
+      </c>
+      <c r="BC58">
+        <v>0</v>
+      </c>
+      <c r="BD58">
+        <v>0</v>
+      </c>
+      <c r="BE58">
+        <v>0</v>
+      </c>
+      <c r="BF58">
+        <v>0</v>
+      </c>
+      <c r="BG58">
+        <v>0</v>
+      </c>
+      <c r="BH58">
+        <v>0</v>
+      </c>
+      <c r="BI58">
+        <v>0</v>
+      </c>
+      <c r="BJ58">
+        <v>0</v>
+      </c>
+      <c r="BK58">
+        <v>0</v>
+      </c>
+      <c r="BL58">
+        <v>0</v>
+      </c>
+      <c r="BM58">
+        <v>0</v>
+      </c>
+      <c r="BN58">
+        <v>0</v>
+      </c>
+      <c r="BO58">
+        <v>0</v>
+      </c>
+      <c r="BP58">
+        <v>0</v>
+      </c>
+      <c r="BQ58">
+        <v>0</v>
+      </c>
+      <c r="BR58">
+        <v>0</v>
+      </c>
+      <c r="BS58">
+        <v>0</v>
+      </c>
+      <c r="BT58">
+        <v>0</v>
+      </c>
+      <c r="BU58">
+        <v>0</v>
+      </c>
+      <c r="BV58">
+        <v>0</v>
+      </c>
+      <c r="BW58">
+        <v>0</v>
+      </c>
+      <c r="BX58">
+        <v>0</v>
+      </c>
+      <c r="BY58">
+        <v>0</v>
+      </c>
+      <c r="BZ58">
+        <v>0</v>
+      </c>
+      <c r="CA58">
+        <v>0</v>
+      </c>
+      <c r="CB58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>438</v>
+      </c>
+      <c r="C59">
+        <v>4</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="I59">
+        <v>0</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>0</v>
+      </c>
+      <c r="L59">
+        <v>0</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+      <c r="N59">
+        <v>0</v>
+      </c>
+      <c r="O59">
+        <v>0</v>
+      </c>
+      <c r="P59">
+        <v>0</v>
+      </c>
+      <c r="Q59">
+        <v>0</v>
+      </c>
+      <c r="R59">
+        <v>0</v>
+      </c>
+      <c r="S59">
+        <v>1</v>
+      </c>
+      <c r="T59">
+        <v>0</v>
+      </c>
+      <c r="U59">
+        <v>0</v>
+      </c>
+      <c r="V59">
+        <v>0</v>
+      </c>
+      <c r="W59">
+        <v>0</v>
+      </c>
+      <c r="X59">
+        <v>0</v>
+      </c>
+      <c r="Y59">
+        <v>0</v>
+      </c>
+      <c r="Z59">
+        <v>0</v>
+      </c>
+      <c r="AA59">
+        <v>0</v>
+      </c>
+      <c r="AB59">
+        <v>0</v>
+      </c>
+      <c r="AC59">
+        <v>0</v>
+      </c>
+      <c r="AD59">
+        <v>0</v>
+      </c>
+      <c r="AE59">
+        <v>0</v>
+      </c>
+      <c r="AF59">
+        <v>0</v>
+      </c>
+      <c r="AG59">
+        <v>0</v>
+      </c>
+      <c r="AH59">
+        <v>0</v>
+      </c>
+      <c r="AI59">
+        <v>0</v>
+      </c>
+      <c r="AJ59">
+        <v>0</v>
+      </c>
+      <c r="AK59">
+        <v>0</v>
+      </c>
+      <c r="AL59">
+        <v>1</v>
+      </c>
+      <c r="AM59">
+        <v>0</v>
+      </c>
+      <c r="AN59">
+        <v>0</v>
+      </c>
+      <c r="AO59">
+        <v>0</v>
+      </c>
+      <c r="AP59">
+        <v>0</v>
+      </c>
+      <c r="AQ59">
+        <v>0</v>
+      </c>
+      <c r="AR59">
+        <v>0</v>
+      </c>
+      <c r="AS59">
+        <v>0</v>
+      </c>
+      <c r="AT59">
+        <v>0</v>
+      </c>
+      <c r="AU59">
+        <v>0</v>
+      </c>
+      <c r="AV59">
+        <v>0</v>
+      </c>
+      <c r="AW59">
+        <v>0</v>
+      </c>
+      <c r="AX59">
+        <v>0</v>
+      </c>
+      <c r="AY59">
+        <v>0</v>
+      </c>
+      <c r="AZ59">
+        <v>0</v>
+      </c>
+      <c r="BA59">
+        <v>0</v>
+      </c>
+      <c r="BB59">
+        <v>0</v>
+      </c>
+      <c r="BC59">
+        <v>0</v>
+      </c>
+      <c r="BD59">
+        <v>0</v>
+      </c>
+      <c r="BE59">
+        <v>0</v>
+      </c>
+      <c r="BF59">
+        <v>0</v>
+      </c>
+      <c r="BG59">
+        <v>0</v>
+      </c>
+      <c r="BH59">
+        <v>0</v>
+      </c>
+      <c r="BI59">
+        <v>0</v>
+      </c>
+      <c r="BJ59">
+        <v>0</v>
+      </c>
+      <c r="BK59">
+        <v>0</v>
+      </c>
+      <c r="BL59">
+        <v>0</v>
+      </c>
+      <c r="BM59">
+        <v>0</v>
+      </c>
+      <c r="BN59">
+        <v>0</v>
+      </c>
+      <c r="BO59">
+        <v>0</v>
+      </c>
+      <c r="BP59">
+        <v>0</v>
+      </c>
+      <c r="BQ59">
+        <v>0</v>
+      </c>
+      <c r="BR59">
+        <v>0</v>
+      </c>
+      <c r="BS59">
+        <v>0</v>
+      </c>
+      <c r="BT59">
+        <v>0</v>
+      </c>
+      <c r="BU59">
+        <v>0</v>
+      </c>
+      <c r="BV59">
+        <v>0</v>
+      </c>
+      <c r="BW59">
+        <v>0</v>
+      </c>
+      <c r="BX59">
+        <v>0</v>
+      </c>
+      <c r="BY59">
+        <v>0</v>
+      </c>
+      <c r="BZ59">
+        <v>0</v>
+      </c>
+      <c r="CA59">
+        <v>0</v>
+      </c>
+      <c r="CB59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>439</v>
+      </c>
+      <c r="C60">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="61" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="62" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>441</v>
+      </c>
+      <c r="C62">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="63" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>444</v>
+      </c>
+      <c r="C63">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>448</v>
+      </c>
+      <c r="C64">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added capture data for a few more lines
</commit_message>
<xml_diff>
--- a/Lovejoy data table_Frequency of capture.xlsx
+++ b/Lovejoy data table_Frequency of capture.xlsx
@@ -480,7 +480,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
+      <selection pane="bottomLeft" activeCell="L49" sqref="L49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11875,6 +11875,39 @@
       <c r="C51">
         <v>28</v>
       </c>
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>1</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>0</v>
+      </c>
+      <c r="N51">
+        <v>1</v>
+      </c>
     </row>
     <row r="52" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A52">
@@ -12600,6 +12633,237 @@
       <c r="C55">
         <v>22</v>
       </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>1</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>5</v>
+      </c>
+      <c r="J55">
+        <v>0</v>
+      </c>
+      <c r="K55">
+        <v>0</v>
+      </c>
+      <c r="L55">
+        <v>0</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+      <c r="N55">
+        <v>0</v>
+      </c>
+      <c r="O55">
+        <v>0</v>
+      </c>
+      <c r="P55">
+        <v>0</v>
+      </c>
+      <c r="Q55">
+        <v>0</v>
+      </c>
+      <c r="R55">
+        <v>0</v>
+      </c>
+      <c r="S55">
+        <v>0</v>
+      </c>
+      <c r="T55">
+        <v>0</v>
+      </c>
+      <c r="U55">
+        <v>1</v>
+      </c>
+      <c r="V55">
+        <v>0</v>
+      </c>
+      <c r="W55">
+        <v>1</v>
+      </c>
+      <c r="X55">
+        <v>0</v>
+      </c>
+      <c r="Y55">
+        <v>1</v>
+      </c>
+      <c r="Z55">
+        <v>1</v>
+      </c>
+      <c r="AA55">
+        <v>1</v>
+      </c>
+      <c r="AB55">
+        <v>1</v>
+      </c>
+      <c r="AC55">
+        <v>2</v>
+      </c>
+      <c r="AD55">
+        <v>0</v>
+      </c>
+      <c r="AE55">
+        <v>0</v>
+      </c>
+      <c r="AF55">
+        <v>0</v>
+      </c>
+      <c r="AG55">
+        <v>1</v>
+      </c>
+      <c r="AH55">
+        <v>0</v>
+      </c>
+      <c r="AI55">
+        <v>1</v>
+      </c>
+      <c r="AJ55">
+        <v>0</v>
+      </c>
+      <c r="AK55">
+        <v>0</v>
+      </c>
+      <c r="AL55">
+        <v>0</v>
+      </c>
+      <c r="AM55">
+        <v>0</v>
+      </c>
+      <c r="AN55">
+        <v>0</v>
+      </c>
+      <c r="AO55">
+        <v>0</v>
+      </c>
+      <c r="AP55">
+        <v>0</v>
+      </c>
+      <c r="AQ55">
+        <v>0</v>
+      </c>
+      <c r="AR55">
+        <v>0</v>
+      </c>
+      <c r="AS55">
+        <v>0</v>
+      </c>
+      <c r="AT55">
+        <v>0</v>
+      </c>
+      <c r="AU55">
+        <v>0</v>
+      </c>
+      <c r="AV55">
+        <v>0</v>
+      </c>
+      <c r="AW55">
+        <v>0</v>
+      </c>
+      <c r="AX55">
+        <v>1</v>
+      </c>
+      <c r="AY55">
+        <v>0</v>
+      </c>
+      <c r="AZ55">
+        <v>0</v>
+      </c>
+      <c r="BA55">
+        <v>0</v>
+      </c>
+      <c r="BB55">
+        <v>0</v>
+      </c>
+      <c r="BC55">
+        <v>0</v>
+      </c>
+      <c r="BD55">
+        <v>0</v>
+      </c>
+      <c r="BE55">
+        <v>0</v>
+      </c>
+      <c r="BF55">
+        <v>0</v>
+      </c>
+      <c r="BG55">
+        <v>0</v>
+      </c>
+      <c r="BH55">
+        <v>0</v>
+      </c>
+      <c r="BI55">
+        <v>1</v>
+      </c>
+      <c r="BJ55">
+        <v>0</v>
+      </c>
+      <c r="BK55">
+        <v>0</v>
+      </c>
+      <c r="BL55">
+        <v>0</v>
+      </c>
+      <c r="BM55">
+        <v>0</v>
+      </c>
+      <c r="BN55">
+        <v>0</v>
+      </c>
+      <c r="BO55">
+        <v>1</v>
+      </c>
+      <c r="BP55">
+        <v>1</v>
+      </c>
+      <c r="BQ55">
+        <v>1</v>
+      </c>
+      <c r="BR55">
+        <v>0</v>
+      </c>
+      <c r="BS55">
+        <v>0</v>
+      </c>
+      <c r="BT55">
+        <v>0</v>
+      </c>
+      <c r="BU55">
+        <v>1</v>
+      </c>
+      <c r="BV55">
+        <v>0</v>
+      </c>
+      <c r="BW55">
+        <v>0</v>
+      </c>
+      <c r="BX55">
+        <v>0</v>
+      </c>
+      <c r="BY55">
+        <v>0</v>
+      </c>
+      <c r="BZ55">
+        <v>0</v>
+      </c>
+      <c r="CA55">
+        <v>0</v>
+      </c>
+      <c r="CB55">
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A56">
@@ -13333,6 +13597,234 @@
       <c r="C60">
         <v>24</v>
       </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>1</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>0</v>
+      </c>
+      <c r="K60">
+        <v>1</v>
+      </c>
+      <c r="L60">
+        <v>0</v>
+      </c>
+      <c r="M60">
+        <v>0</v>
+      </c>
+      <c r="N60">
+        <v>0</v>
+      </c>
+      <c r="O60">
+        <v>0</v>
+      </c>
+      <c r="P60">
+        <v>0</v>
+      </c>
+      <c r="Q60">
+        <v>0</v>
+      </c>
+      <c r="R60">
+        <v>1</v>
+      </c>
+      <c r="S60">
+        <v>0</v>
+      </c>
+      <c r="T60">
+        <v>0</v>
+      </c>
+      <c r="U60">
+        <v>0</v>
+      </c>
+      <c r="V60">
+        <v>0</v>
+      </c>
+      <c r="W60">
+        <v>0</v>
+      </c>
+      <c r="X60">
+        <v>0</v>
+      </c>
+      <c r="Y60">
+        <v>1</v>
+      </c>
+      <c r="Z60">
+        <v>0</v>
+      </c>
+      <c r="AA60">
+        <v>0</v>
+      </c>
+      <c r="AB60">
+        <v>0</v>
+      </c>
+      <c r="AC60">
+        <v>2</v>
+      </c>
+      <c r="AD60">
+        <v>0</v>
+      </c>
+      <c r="AE60">
+        <v>1</v>
+      </c>
+      <c r="AF60">
+        <v>0</v>
+      </c>
+      <c r="AG60">
+        <v>0</v>
+      </c>
+      <c r="AI60">
+        <v>1</v>
+      </c>
+      <c r="AJ60">
+        <v>0</v>
+      </c>
+      <c r="AK60">
+        <v>0</v>
+      </c>
+      <c r="AL60">
+        <v>0</v>
+      </c>
+      <c r="AM60">
+        <v>0</v>
+      </c>
+      <c r="AN60">
+        <v>0</v>
+      </c>
+      <c r="AO60">
+        <v>1</v>
+      </c>
+      <c r="AP60">
+        <v>0</v>
+      </c>
+      <c r="AQ60">
+        <v>0</v>
+      </c>
+      <c r="AR60">
+        <v>0</v>
+      </c>
+      <c r="AS60">
+        <v>1</v>
+      </c>
+      <c r="AT60">
+        <v>1</v>
+      </c>
+      <c r="AU60">
+        <v>2</v>
+      </c>
+      <c r="AV60">
+        <v>0</v>
+      </c>
+      <c r="AW60">
+        <v>1</v>
+      </c>
+      <c r="AX60">
+        <v>0</v>
+      </c>
+      <c r="AY60">
+        <v>0</v>
+      </c>
+      <c r="AZ60">
+        <v>0</v>
+      </c>
+      <c r="BA60">
+        <v>2</v>
+      </c>
+      <c r="BB60">
+        <v>3</v>
+      </c>
+      <c r="BC60">
+        <v>1</v>
+      </c>
+      <c r="BD60">
+        <v>2</v>
+      </c>
+      <c r="BE60">
+        <v>1</v>
+      </c>
+      <c r="BF60">
+        <v>0</v>
+      </c>
+      <c r="BG60">
+        <v>0</v>
+      </c>
+      <c r="BH60">
+        <v>0</v>
+      </c>
+      <c r="BI60">
+        <v>0</v>
+      </c>
+      <c r="BJ60">
+        <v>0</v>
+      </c>
+      <c r="BK60">
+        <v>0</v>
+      </c>
+      <c r="BL60">
+        <v>0</v>
+      </c>
+      <c r="BM60">
+        <v>0</v>
+      </c>
+      <c r="BN60">
+        <v>0</v>
+      </c>
+      <c r="BO60">
+        <v>0</v>
+      </c>
+      <c r="BP60">
+        <v>0</v>
+      </c>
+      <c r="BQ60">
+        <v>0</v>
+      </c>
+      <c r="BR60">
+        <v>0</v>
+      </c>
+      <c r="BS60">
+        <v>0</v>
+      </c>
+      <c r="BT60">
+        <v>0</v>
+      </c>
+      <c r="BU60">
+        <v>0</v>
+      </c>
+      <c r="BV60">
+        <v>0</v>
+      </c>
+      <c r="BW60">
+        <v>0</v>
+      </c>
+      <c r="BX60">
+        <v>0</v>
+      </c>
+      <c r="BY60">
+        <v>0</v>
+      </c>
+      <c r="BZ60">
+        <v>0</v>
+      </c>
+      <c r="CA60">
+        <v>0</v>
+      </c>
+      <c r="CB60">
+        <v>0</v>
+      </c>
     </row>
     <row r="61" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A61">
@@ -13353,6 +13845,237 @@
       </c>
       <c r="C63">
         <v>14</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>1</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>1</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+      <c r="I63">
+        <v>2</v>
+      </c>
+      <c r="J63">
+        <v>2</v>
+      </c>
+      <c r="K63">
+        <v>0</v>
+      </c>
+      <c r="L63">
+        <v>2</v>
+      </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+      <c r="N63">
+        <v>0</v>
+      </c>
+      <c r="O63">
+        <v>0</v>
+      </c>
+      <c r="P63">
+        <v>1</v>
+      </c>
+      <c r="Q63">
+        <v>1</v>
+      </c>
+      <c r="R63">
+        <v>0</v>
+      </c>
+      <c r="S63">
+        <v>0</v>
+      </c>
+      <c r="T63">
+        <v>0</v>
+      </c>
+      <c r="U63">
+        <v>0</v>
+      </c>
+      <c r="V63">
+        <v>0</v>
+      </c>
+      <c r="W63">
+        <v>0</v>
+      </c>
+      <c r="X63">
+        <v>2</v>
+      </c>
+      <c r="Y63">
+        <v>0</v>
+      </c>
+      <c r="Z63">
+        <v>0</v>
+      </c>
+      <c r="AA63">
+        <v>0</v>
+      </c>
+      <c r="AB63">
+        <v>0</v>
+      </c>
+      <c r="AC63">
+        <v>0</v>
+      </c>
+      <c r="AD63">
+        <v>0</v>
+      </c>
+      <c r="AE63">
+        <v>0</v>
+      </c>
+      <c r="AF63">
+        <v>0</v>
+      </c>
+      <c r="AG63">
+        <v>0</v>
+      </c>
+      <c r="AH63">
+        <v>0</v>
+      </c>
+      <c r="AI63">
+        <v>0</v>
+      </c>
+      <c r="AJ63">
+        <v>0</v>
+      </c>
+      <c r="AK63">
+        <v>1</v>
+      </c>
+      <c r="AL63">
+        <v>0</v>
+      </c>
+      <c r="AM63">
+        <v>0</v>
+      </c>
+      <c r="AN63">
+        <v>0</v>
+      </c>
+      <c r="AO63">
+        <v>0</v>
+      </c>
+      <c r="AP63">
+        <v>0</v>
+      </c>
+      <c r="AQ63">
+        <v>0</v>
+      </c>
+      <c r="AR63">
+        <v>0</v>
+      </c>
+      <c r="AS63">
+        <v>0</v>
+      </c>
+      <c r="AT63">
+        <v>0</v>
+      </c>
+      <c r="AU63">
+        <v>0</v>
+      </c>
+      <c r="AV63">
+        <v>0</v>
+      </c>
+      <c r="AW63">
+        <v>0</v>
+      </c>
+      <c r="AX63">
+        <v>0</v>
+      </c>
+      <c r="AY63">
+        <v>0</v>
+      </c>
+      <c r="AZ63">
+        <v>0</v>
+      </c>
+      <c r="BA63">
+        <v>0</v>
+      </c>
+      <c r="BB63">
+        <v>0</v>
+      </c>
+      <c r="BC63">
+        <v>0</v>
+      </c>
+      <c r="BD63">
+        <v>0</v>
+      </c>
+      <c r="BE63">
+        <v>0</v>
+      </c>
+      <c r="BF63">
+        <v>0</v>
+      </c>
+      <c r="BG63">
+        <v>0</v>
+      </c>
+      <c r="BH63">
+        <v>0</v>
+      </c>
+      <c r="BI63">
+        <v>0</v>
+      </c>
+      <c r="BJ63">
+        <v>0</v>
+      </c>
+      <c r="BK63">
+        <v>0</v>
+      </c>
+      <c r="BL63">
+        <v>0</v>
+      </c>
+      <c r="BM63">
+        <v>0</v>
+      </c>
+      <c r="BN63">
+        <v>0</v>
+      </c>
+      <c r="BO63">
+        <v>0</v>
+      </c>
+      <c r="BP63">
+        <v>0</v>
+      </c>
+      <c r="BQ63">
+        <v>0</v>
+      </c>
+      <c r="BR63">
+        <v>0</v>
+      </c>
+      <c r="BS63">
+        <v>0</v>
+      </c>
+      <c r="BT63">
+        <v>0</v>
+      </c>
+      <c r="BU63">
+        <v>0</v>
+      </c>
+      <c r="BV63">
+        <v>0</v>
+      </c>
+      <c r="BW63">
+        <v>0</v>
+      </c>
+      <c r="BX63">
+        <v>0</v>
+      </c>
+      <c r="BY63">
+        <v>0</v>
+      </c>
+      <c r="BZ63">
+        <v>0</v>
+      </c>
+      <c r="CA63">
+        <v>0</v>
+      </c>
+      <c r="CB63">
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:80" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
adding final capture data counts for pg. 180
</commit_message>
<xml_diff>
--- a/Lovejoy data table_Frequency of capture.xlsx
+++ b/Lovejoy data table_Frequency of capture.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -480,7 +478,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L49" sqref="L49"/>
+      <selection pane="bottomLeft" activeCell="H78" sqref="H78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10656,6 +10654,237 @@
       <c r="C43">
         <v>217</v>
       </c>
+      <c r="D43">
+        <v>5</v>
+      </c>
+      <c r="E43">
+        <v>7</v>
+      </c>
+      <c r="F43">
+        <v>5</v>
+      </c>
+      <c r="G43">
+        <v>6</v>
+      </c>
+      <c r="H43">
+        <v>8</v>
+      </c>
+      <c r="I43">
+        <v>4</v>
+      </c>
+      <c r="J43">
+        <v>5</v>
+      </c>
+      <c r="K43">
+        <v>2</v>
+      </c>
+      <c r="L43">
+        <v>5</v>
+      </c>
+      <c r="M43">
+        <v>3</v>
+      </c>
+      <c r="N43">
+        <v>1</v>
+      </c>
+      <c r="O43">
+        <v>2</v>
+      </c>
+      <c r="P43">
+        <v>3</v>
+      </c>
+      <c r="Q43">
+        <v>1</v>
+      </c>
+      <c r="R43">
+        <v>6</v>
+      </c>
+      <c r="S43">
+        <v>1</v>
+      </c>
+      <c r="T43">
+        <v>1</v>
+      </c>
+      <c r="U43">
+        <v>3</v>
+      </c>
+      <c r="V43">
+        <v>1</v>
+      </c>
+      <c r="W43">
+        <v>3</v>
+      </c>
+      <c r="X43">
+        <v>2</v>
+      </c>
+      <c r="Y43">
+        <v>0</v>
+      </c>
+      <c r="Z43">
+        <v>1</v>
+      </c>
+      <c r="AA43">
+        <v>3</v>
+      </c>
+      <c r="AB43">
+        <v>2</v>
+      </c>
+      <c r="AC43">
+        <v>2</v>
+      </c>
+      <c r="AD43">
+        <v>5</v>
+      </c>
+      <c r="AE43">
+        <v>5</v>
+      </c>
+      <c r="AF43">
+        <v>3</v>
+      </c>
+      <c r="AG43">
+        <v>2</v>
+      </c>
+      <c r="AH43">
+        <v>4</v>
+      </c>
+      <c r="AI43">
+        <v>4</v>
+      </c>
+      <c r="AJ43">
+        <v>3</v>
+      </c>
+      <c r="AK43">
+        <v>2</v>
+      </c>
+      <c r="AL43">
+        <v>2</v>
+      </c>
+      <c r="AM43">
+        <v>2</v>
+      </c>
+      <c r="AN43">
+        <v>4</v>
+      </c>
+      <c r="AO43">
+        <v>2</v>
+      </c>
+      <c r="AP43">
+        <v>0</v>
+      </c>
+      <c r="AQ43">
+        <v>2</v>
+      </c>
+      <c r="AR43">
+        <v>5</v>
+      </c>
+      <c r="AS43">
+        <v>2</v>
+      </c>
+      <c r="AT43">
+        <v>3</v>
+      </c>
+      <c r="AU43">
+        <v>3</v>
+      </c>
+      <c r="AV43">
+        <v>2</v>
+      </c>
+      <c r="AW43">
+        <v>3</v>
+      </c>
+      <c r="AX43">
+        <v>2</v>
+      </c>
+      <c r="AY43">
+        <v>4</v>
+      </c>
+      <c r="AZ43">
+        <v>3</v>
+      </c>
+      <c r="BA43">
+        <v>4</v>
+      </c>
+      <c r="BB43">
+        <v>5</v>
+      </c>
+      <c r="BC43">
+        <v>4</v>
+      </c>
+      <c r="BD43">
+        <v>5</v>
+      </c>
+      <c r="BE43">
+        <v>4</v>
+      </c>
+      <c r="BF43">
+        <v>2</v>
+      </c>
+      <c r="BG43">
+        <v>0</v>
+      </c>
+      <c r="BH43">
+        <v>1</v>
+      </c>
+      <c r="BI43">
+        <v>0</v>
+      </c>
+      <c r="BJ43">
+        <v>2</v>
+      </c>
+      <c r="BK43">
+        <v>1</v>
+      </c>
+      <c r="BL43">
+        <v>0</v>
+      </c>
+      <c r="BM43">
+        <v>2</v>
+      </c>
+      <c r="BN43">
+        <v>3</v>
+      </c>
+      <c r="BO43">
+        <v>0</v>
+      </c>
+      <c r="BP43">
+        <v>3</v>
+      </c>
+      <c r="BQ43">
+        <v>2</v>
+      </c>
+      <c r="BR43">
+        <v>1</v>
+      </c>
+      <c r="BS43">
+        <v>2</v>
+      </c>
+      <c r="BT43">
+        <v>5</v>
+      </c>
+      <c r="BU43">
+        <v>3</v>
+      </c>
+      <c r="BV43">
+        <v>4</v>
+      </c>
+      <c r="BW43">
+        <v>3</v>
+      </c>
+      <c r="BX43">
+        <v>0</v>
+      </c>
+      <c r="BY43">
+        <v>5</v>
+      </c>
+      <c r="BZ43">
+        <v>1</v>
+      </c>
+      <c r="CA43">
+        <v>6</v>
+      </c>
+      <c r="CB43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A44">
@@ -11381,6 +11610,237 @@
       <c r="C47">
         <v>41</v>
       </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>1</v>
+      </c>
+      <c r="J47">
+        <v>1</v>
+      </c>
+      <c r="K47">
+        <v>1</v>
+      </c>
+      <c r="L47">
+        <v>2</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+      <c r="P47">
+        <v>3</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>0</v>
+      </c>
+      <c r="T47">
+        <v>0</v>
+      </c>
+      <c r="U47">
+        <v>0</v>
+      </c>
+      <c r="V47">
+        <v>1</v>
+      </c>
+      <c r="W47">
+        <v>0</v>
+      </c>
+      <c r="X47">
+        <v>0</v>
+      </c>
+      <c r="Y47">
+        <v>2</v>
+      </c>
+      <c r="Z47">
+        <v>0</v>
+      </c>
+      <c r="AA47">
+        <v>1</v>
+      </c>
+      <c r="AB47">
+        <v>0</v>
+      </c>
+      <c r="AC47">
+        <v>0</v>
+      </c>
+      <c r="AD47">
+        <v>2</v>
+      </c>
+      <c r="AE47">
+        <v>1</v>
+      </c>
+      <c r="AF47">
+        <v>2</v>
+      </c>
+      <c r="AG47">
+        <v>1</v>
+      </c>
+      <c r="AH47">
+        <v>0</v>
+      </c>
+      <c r="AI47">
+        <v>2</v>
+      </c>
+      <c r="AJ47">
+        <v>0</v>
+      </c>
+      <c r="AK47">
+        <v>0</v>
+      </c>
+      <c r="AL47">
+        <v>1</v>
+      </c>
+      <c r="AM47">
+        <v>0</v>
+      </c>
+      <c r="AN47">
+        <v>1</v>
+      </c>
+      <c r="AO47">
+        <v>1</v>
+      </c>
+      <c r="AP47">
+        <v>0</v>
+      </c>
+      <c r="AQ47">
+        <v>0</v>
+      </c>
+      <c r="AR47">
+        <v>0</v>
+      </c>
+      <c r="AS47">
+        <v>0</v>
+      </c>
+      <c r="AT47">
+        <v>0</v>
+      </c>
+      <c r="AU47">
+        <v>4</v>
+      </c>
+      <c r="AV47">
+        <v>2</v>
+      </c>
+      <c r="AW47">
+        <v>0</v>
+      </c>
+      <c r="AX47">
+        <v>2</v>
+      </c>
+      <c r="AY47">
+        <v>0</v>
+      </c>
+      <c r="AZ47">
+        <v>1</v>
+      </c>
+      <c r="BA47">
+        <v>0</v>
+      </c>
+      <c r="BB47">
+        <v>0</v>
+      </c>
+      <c r="BC47">
+        <v>1</v>
+      </c>
+      <c r="BD47">
+        <v>0</v>
+      </c>
+      <c r="BE47">
+        <v>0</v>
+      </c>
+      <c r="BF47">
+        <v>0</v>
+      </c>
+      <c r="BG47">
+        <v>0</v>
+      </c>
+      <c r="BH47">
+        <v>0</v>
+      </c>
+      <c r="BI47">
+        <v>0</v>
+      </c>
+      <c r="BJ47">
+        <v>0</v>
+      </c>
+      <c r="BK47">
+        <v>0</v>
+      </c>
+      <c r="BL47">
+        <v>0</v>
+      </c>
+      <c r="BM47">
+        <v>0</v>
+      </c>
+      <c r="BN47">
+        <v>0</v>
+      </c>
+      <c r="BO47">
+        <v>1</v>
+      </c>
+      <c r="BP47">
+        <v>0</v>
+      </c>
+      <c r="BQ47">
+        <v>0</v>
+      </c>
+      <c r="BR47">
+        <v>0</v>
+      </c>
+      <c r="BS47">
+        <v>0</v>
+      </c>
+      <c r="BT47">
+        <v>0</v>
+      </c>
+      <c r="BU47">
+        <v>0</v>
+      </c>
+      <c r="BV47">
+        <v>0</v>
+      </c>
+      <c r="BW47">
+        <v>0</v>
+      </c>
+      <c r="BX47">
+        <v>0</v>
+      </c>
+      <c r="BY47">
+        <v>0</v>
+      </c>
+      <c r="BZ47">
+        <v>1</v>
+      </c>
+      <c r="CA47">
+        <v>0</v>
+      </c>
+      <c r="CB47">
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A48">
@@ -11389,6 +11849,237 @@
       <c r="C48">
         <v>162</v>
       </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>3</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>3</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+      <c r="P48">
+        <v>1</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>0</v>
+      </c>
+      <c r="T48">
+        <v>2</v>
+      </c>
+      <c r="U48">
+        <v>2</v>
+      </c>
+      <c r="V48">
+        <v>1</v>
+      </c>
+      <c r="W48">
+        <v>1</v>
+      </c>
+      <c r="X48">
+        <v>0</v>
+      </c>
+      <c r="Y48">
+        <v>1</v>
+      </c>
+      <c r="Z48">
+        <v>0</v>
+      </c>
+      <c r="AA48">
+        <v>0</v>
+      </c>
+      <c r="AB48">
+        <v>0</v>
+      </c>
+      <c r="AC48">
+        <v>5</v>
+      </c>
+      <c r="AD48">
+        <v>3</v>
+      </c>
+      <c r="AE48">
+        <v>2</v>
+      </c>
+      <c r="AF48">
+        <v>3</v>
+      </c>
+      <c r="AG48">
+        <v>2</v>
+      </c>
+      <c r="AH48">
+        <v>2</v>
+      </c>
+      <c r="AI48">
+        <v>9</v>
+      </c>
+      <c r="AJ48">
+        <v>4</v>
+      </c>
+      <c r="AK48">
+        <v>0</v>
+      </c>
+      <c r="AL48">
+        <v>3</v>
+      </c>
+      <c r="AM48">
+        <v>1</v>
+      </c>
+      <c r="AN48">
+        <v>2</v>
+      </c>
+      <c r="AO48">
+        <v>0</v>
+      </c>
+      <c r="AP48">
+        <v>3</v>
+      </c>
+      <c r="AQ48">
+        <v>1</v>
+      </c>
+      <c r="AR48">
+        <v>1</v>
+      </c>
+      <c r="AS48">
+        <v>1</v>
+      </c>
+      <c r="AT48">
+        <v>0</v>
+      </c>
+      <c r="AU48">
+        <v>8</v>
+      </c>
+      <c r="AV48">
+        <v>4</v>
+      </c>
+      <c r="AW48">
+        <v>4</v>
+      </c>
+      <c r="AX48">
+        <v>13</v>
+      </c>
+      <c r="AY48">
+        <v>7</v>
+      </c>
+      <c r="AZ48">
+        <v>13</v>
+      </c>
+      <c r="BA48">
+        <v>5</v>
+      </c>
+      <c r="BB48">
+        <v>16</v>
+      </c>
+      <c r="BC48">
+        <v>9</v>
+      </c>
+      <c r="BD48">
+        <v>4</v>
+      </c>
+      <c r="BE48">
+        <v>4</v>
+      </c>
+      <c r="BF48">
+        <v>0</v>
+      </c>
+      <c r="BG48">
+        <v>1</v>
+      </c>
+      <c r="BH48">
+        <v>0</v>
+      </c>
+      <c r="BI48">
+        <v>0</v>
+      </c>
+      <c r="BJ48">
+        <v>2</v>
+      </c>
+      <c r="BK48">
+        <v>1</v>
+      </c>
+      <c r="BL48">
+        <v>1</v>
+      </c>
+      <c r="BM48">
+        <v>4</v>
+      </c>
+      <c r="BN48">
+        <v>0</v>
+      </c>
+      <c r="BO48">
+        <v>0</v>
+      </c>
+      <c r="BP48">
+        <v>1</v>
+      </c>
+      <c r="BQ48">
+        <v>1</v>
+      </c>
+      <c r="BR48">
+        <v>0</v>
+      </c>
+      <c r="BS48">
+        <v>1</v>
+      </c>
+      <c r="BT48">
+        <v>1</v>
+      </c>
+      <c r="BU48">
+        <v>2</v>
+      </c>
+      <c r="BV48">
+        <v>0</v>
+      </c>
+      <c r="BW48">
+        <v>1</v>
+      </c>
+      <c r="BX48">
+        <v>0</v>
+      </c>
+      <c r="BY48">
+        <v>0</v>
+      </c>
+      <c r="BZ48">
+        <v>0</v>
+      </c>
+      <c r="CA48">
+        <v>0</v>
+      </c>
+      <c r="CB48">
+        <v>2</v>
+      </c>
     </row>
     <row r="49" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A49">
@@ -11908,6 +12599,204 @@
       <c r="N51">
         <v>1</v>
       </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="Q51">
+        <v>0</v>
+      </c>
+      <c r="R51">
+        <v>1</v>
+      </c>
+      <c r="S51">
+        <v>1</v>
+      </c>
+      <c r="T51">
+        <v>0</v>
+      </c>
+      <c r="U51">
+        <v>0</v>
+      </c>
+      <c r="V51">
+        <v>0</v>
+      </c>
+      <c r="W51">
+        <v>1</v>
+      </c>
+      <c r="X51">
+        <v>1</v>
+      </c>
+      <c r="Y51">
+        <v>0</v>
+      </c>
+      <c r="Z51">
+        <v>0</v>
+      </c>
+      <c r="AA51">
+        <v>0</v>
+      </c>
+      <c r="AB51">
+        <v>0</v>
+      </c>
+      <c r="AC51">
+        <v>0</v>
+      </c>
+      <c r="AD51">
+        <v>2</v>
+      </c>
+      <c r="AE51">
+        <v>1</v>
+      </c>
+      <c r="AF51">
+        <v>1</v>
+      </c>
+      <c r="AG51">
+        <v>0</v>
+      </c>
+      <c r="AH51">
+        <v>3</v>
+      </c>
+      <c r="AI51">
+        <v>0</v>
+      </c>
+      <c r="AJ51">
+        <v>0</v>
+      </c>
+      <c r="AK51">
+        <v>0</v>
+      </c>
+      <c r="AL51">
+        <v>0</v>
+      </c>
+      <c r="AM51">
+        <v>0</v>
+      </c>
+      <c r="AN51">
+        <v>1</v>
+      </c>
+      <c r="AO51">
+        <v>0</v>
+      </c>
+      <c r="AP51">
+        <v>0</v>
+      </c>
+      <c r="AQ51">
+        <v>0</v>
+      </c>
+      <c r="AR51">
+        <v>2</v>
+      </c>
+      <c r="AS51">
+        <v>1</v>
+      </c>
+      <c r="AT51">
+        <v>1</v>
+      </c>
+      <c r="AU51">
+        <v>0</v>
+      </c>
+      <c r="AV51">
+        <v>1</v>
+      </c>
+      <c r="AW51">
+        <v>2</v>
+      </c>
+      <c r="AX51">
+        <v>0</v>
+      </c>
+      <c r="AY51">
+        <v>0</v>
+      </c>
+      <c r="AZ51">
+        <v>1</v>
+      </c>
+      <c r="BA51">
+        <v>1</v>
+      </c>
+      <c r="BB51">
+        <v>1</v>
+      </c>
+      <c r="BC51">
+        <v>1</v>
+      </c>
+      <c r="BD51">
+        <v>1</v>
+      </c>
+      <c r="BE51">
+        <v>0</v>
+      </c>
+      <c r="BF51">
+        <v>0</v>
+      </c>
+      <c r="BG51">
+        <v>0</v>
+      </c>
+      <c r="BH51">
+        <v>0</v>
+      </c>
+      <c r="BI51">
+        <v>0</v>
+      </c>
+      <c r="BJ51">
+        <v>0</v>
+      </c>
+      <c r="BK51">
+        <v>0</v>
+      </c>
+      <c r="BL51">
+        <v>0</v>
+      </c>
+      <c r="BM51">
+        <v>0</v>
+      </c>
+      <c r="BN51">
+        <v>0</v>
+      </c>
+      <c r="BO51">
+        <v>0</v>
+      </c>
+      <c r="BP51">
+        <v>0</v>
+      </c>
+      <c r="BQ51">
+        <v>0</v>
+      </c>
+      <c r="BR51">
+        <v>0</v>
+      </c>
+      <c r="BS51">
+        <v>0</v>
+      </c>
+      <c r="BT51">
+        <v>0</v>
+      </c>
+      <c r="BU51">
+        <v>0</v>
+      </c>
+      <c r="BV51">
+        <v>0</v>
+      </c>
+      <c r="BW51">
+        <v>1</v>
+      </c>
+      <c r="BX51">
+        <v>0</v>
+      </c>
+      <c r="BY51">
+        <v>0</v>
+      </c>
+      <c r="BZ51">
+        <v>0</v>
+      </c>
+      <c r="CA51">
+        <v>0</v>
+      </c>
+      <c r="CB51">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A52">
@@ -13111,6 +14000,237 @@
       <c r="C57">
         <v>189</v>
       </c>
+      <c r="D57">
+        <v>4</v>
+      </c>
+      <c r="E57">
+        <v>2</v>
+      </c>
+      <c r="F57">
+        <v>2</v>
+      </c>
+      <c r="G57">
+        <v>1</v>
+      </c>
+      <c r="H57">
+        <v>1</v>
+      </c>
+      <c r="I57">
+        <v>1</v>
+      </c>
+      <c r="J57">
+        <v>2</v>
+      </c>
+      <c r="K57">
+        <v>2</v>
+      </c>
+      <c r="L57">
+        <v>3</v>
+      </c>
+      <c r="M57">
+        <v>1</v>
+      </c>
+      <c r="N57">
+        <v>0</v>
+      </c>
+      <c r="O57">
+        <v>1</v>
+      </c>
+      <c r="P57">
+        <v>0</v>
+      </c>
+      <c r="Q57">
+        <v>0</v>
+      </c>
+      <c r="R57">
+        <v>0</v>
+      </c>
+      <c r="S57">
+        <v>6</v>
+      </c>
+      <c r="T57">
+        <v>2</v>
+      </c>
+      <c r="U57">
+        <v>0</v>
+      </c>
+      <c r="V57">
+        <v>0</v>
+      </c>
+      <c r="W57">
+        <v>0</v>
+      </c>
+      <c r="X57">
+        <v>0</v>
+      </c>
+      <c r="Y57">
+        <v>2</v>
+      </c>
+      <c r="Z57">
+        <v>0</v>
+      </c>
+      <c r="AA57">
+        <v>2</v>
+      </c>
+      <c r="AB57">
+        <v>1</v>
+      </c>
+      <c r="AC57">
+        <v>4</v>
+      </c>
+      <c r="AD57">
+        <v>7</v>
+      </c>
+      <c r="AE57">
+        <v>10</v>
+      </c>
+      <c r="AF57">
+        <v>6</v>
+      </c>
+      <c r="AG57">
+        <v>0</v>
+      </c>
+      <c r="AH57">
+        <v>3</v>
+      </c>
+      <c r="AI57">
+        <v>11</v>
+      </c>
+      <c r="AJ57">
+        <v>1</v>
+      </c>
+      <c r="AK57">
+        <v>2</v>
+      </c>
+      <c r="AL57">
+        <v>0</v>
+      </c>
+      <c r="AM57">
+        <v>0</v>
+      </c>
+      <c r="AN57">
+        <v>3</v>
+      </c>
+      <c r="AO57">
+        <v>1</v>
+      </c>
+      <c r="AP57">
+        <v>4</v>
+      </c>
+      <c r="AQ57">
+        <v>6</v>
+      </c>
+      <c r="AR57">
+        <v>9</v>
+      </c>
+      <c r="AS57">
+        <v>5</v>
+      </c>
+      <c r="AT57">
+        <v>0</v>
+      </c>
+      <c r="AU57">
+        <v>12</v>
+      </c>
+      <c r="AV57">
+        <v>2</v>
+      </c>
+      <c r="AW57">
+        <v>3</v>
+      </c>
+      <c r="AX57">
+        <v>6</v>
+      </c>
+      <c r="AY57">
+        <v>13</v>
+      </c>
+      <c r="AZ57">
+        <v>13</v>
+      </c>
+      <c r="BA57">
+        <v>2</v>
+      </c>
+      <c r="BB57">
+        <v>7</v>
+      </c>
+      <c r="BC57">
+        <v>6</v>
+      </c>
+      <c r="BD57">
+        <v>0</v>
+      </c>
+      <c r="BE57">
+        <v>1</v>
+      </c>
+      <c r="BF57">
+        <v>0</v>
+      </c>
+      <c r="BG57">
+        <v>0</v>
+      </c>
+      <c r="BH57">
+        <v>0</v>
+      </c>
+      <c r="BI57">
+        <v>0</v>
+      </c>
+      <c r="BJ57">
+        <v>0</v>
+      </c>
+      <c r="BK57">
+        <v>1</v>
+      </c>
+      <c r="BL57">
+        <v>0</v>
+      </c>
+      <c r="BM57">
+        <v>2</v>
+      </c>
+      <c r="BN57">
+        <v>0</v>
+      </c>
+      <c r="BO57">
+        <v>0</v>
+      </c>
+      <c r="BP57">
+        <v>0</v>
+      </c>
+      <c r="BQ57">
+        <v>0</v>
+      </c>
+      <c r="BR57">
+        <v>0</v>
+      </c>
+      <c r="BS57">
+        <v>0</v>
+      </c>
+      <c r="BT57">
+        <v>1</v>
+      </c>
+      <c r="BU57">
+        <v>11</v>
+      </c>
+      <c r="BV57">
+        <v>0</v>
+      </c>
+      <c r="BW57">
+        <v>0</v>
+      </c>
+      <c r="BX57">
+        <v>0</v>
+      </c>
+      <c r="BY57">
+        <v>0</v>
+      </c>
+      <c r="BZ57">
+        <v>2</v>
+      </c>
+      <c r="CA57">
+        <v>2</v>
+      </c>
+      <c r="CB57">
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A58">
@@ -13687,6 +14807,9 @@
       <c r="AG60">
         <v>0</v>
       </c>
+      <c r="AH60">
+        <v>0</v>
+      </c>
       <c r="AI60">
         <v>1</v>
       </c>
@@ -13830,6 +14953,240 @@
       <c r="A61">
         <v>440</v>
       </c>
+      <c r="C61">
+        <v>89</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="E61">
+        <v>1</v>
+      </c>
+      <c r="F61">
+        <v>1</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+      <c r="I61">
+        <v>0</v>
+      </c>
+      <c r="J61">
+        <v>1</v>
+      </c>
+      <c r="K61">
+        <v>2</v>
+      </c>
+      <c r="L61">
+        <v>0</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+      <c r="N61">
+        <v>0</v>
+      </c>
+      <c r="O61">
+        <v>1</v>
+      </c>
+      <c r="P61">
+        <v>0</v>
+      </c>
+      <c r="Q61">
+        <v>1</v>
+      </c>
+      <c r="R61">
+        <v>1</v>
+      </c>
+      <c r="S61">
+        <v>1</v>
+      </c>
+      <c r="T61">
+        <v>0</v>
+      </c>
+      <c r="U61">
+        <v>1</v>
+      </c>
+      <c r="V61">
+        <v>0</v>
+      </c>
+      <c r="W61">
+        <v>1</v>
+      </c>
+      <c r="X61">
+        <v>0</v>
+      </c>
+      <c r="Y61">
+        <v>0</v>
+      </c>
+      <c r="Z61">
+        <v>0</v>
+      </c>
+      <c r="AA61">
+        <v>0</v>
+      </c>
+      <c r="AB61">
+        <v>0</v>
+      </c>
+      <c r="AC61">
+        <v>4</v>
+      </c>
+      <c r="AD61">
+        <v>0</v>
+      </c>
+      <c r="AE61">
+        <v>5</v>
+      </c>
+      <c r="AF61">
+        <v>4</v>
+      </c>
+      <c r="AG61">
+        <v>1</v>
+      </c>
+      <c r="AH61">
+        <v>3</v>
+      </c>
+      <c r="AI61">
+        <v>5</v>
+      </c>
+      <c r="AJ61">
+        <v>3</v>
+      </c>
+      <c r="AK61">
+        <v>0</v>
+      </c>
+      <c r="AL61">
+        <v>1</v>
+      </c>
+      <c r="AM61">
+        <v>0</v>
+      </c>
+      <c r="AN61">
+        <v>3</v>
+      </c>
+      <c r="AO61">
+        <v>2</v>
+      </c>
+      <c r="AP61">
+        <v>2</v>
+      </c>
+      <c r="AQ61">
+        <v>2</v>
+      </c>
+      <c r="AR61">
+        <v>0</v>
+      </c>
+      <c r="AS61">
+        <v>0</v>
+      </c>
+      <c r="AT61">
+        <v>0</v>
+      </c>
+      <c r="AU61">
+        <v>3</v>
+      </c>
+      <c r="AV61">
+        <v>3</v>
+      </c>
+      <c r="AW61">
+        <v>4</v>
+      </c>
+      <c r="AX61">
+        <v>3</v>
+      </c>
+      <c r="AY61">
+        <v>3</v>
+      </c>
+      <c r="AZ61">
+        <v>5</v>
+      </c>
+      <c r="BA61">
+        <v>4</v>
+      </c>
+      <c r="BB61">
+        <v>2</v>
+      </c>
+      <c r="BC61">
+        <v>2</v>
+      </c>
+      <c r="BD61">
+        <v>2</v>
+      </c>
+      <c r="BE61">
+        <v>1</v>
+      </c>
+      <c r="BF61">
+        <v>0</v>
+      </c>
+      <c r="BG61">
+        <v>0</v>
+      </c>
+      <c r="BH61">
+        <v>0</v>
+      </c>
+      <c r="BI61">
+        <v>0</v>
+      </c>
+      <c r="BJ61">
+        <v>0</v>
+      </c>
+      <c r="BK61">
+        <v>0</v>
+      </c>
+      <c r="BL61">
+        <v>0</v>
+      </c>
+      <c r="BM61">
+        <v>0</v>
+      </c>
+      <c r="BN61">
+        <v>0</v>
+      </c>
+      <c r="BO61">
+        <v>0</v>
+      </c>
+      <c r="BP61">
+        <v>1</v>
+      </c>
+      <c r="BQ61">
+        <v>0</v>
+      </c>
+      <c r="BR61">
+        <v>0</v>
+      </c>
+      <c r="BS61">
+        <v>3</v>
+      </c>
+      <c r="BT61">
+        <v>1</v>
+      </c>
+      <c r="BU61">
+        <v>1</v>
+      </c>
+      <c r="BV61">
+        <v>0</v>
+      </c>
+      <c r="BW61">
+        <v>1</v>
+      </c>
+      <c r="BX61">
+        <v>0</v>
+      </c>
+      <c r="BY61">
+        <v>0</v>
+      </c>
+      <c r="BZ61">
+        <v>1</v>
+      </c>
+      <c r="CA61">
+        <v>0</v>
+      </c>
+      <c r="CB61">
+        <v>0</v>
+      </c>
     </row>
     <row r="62" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A62">
@@ -13837,6 +15194,237 @@
       </c>
       <c r="C62">
         <v>242</v>
+      </c>
+      <c r="D62">
+        <v>2</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+      <c r="F62">
+        <v>1</v>
+      </c>
+      <c r="G62">
+        <v>9</v>
+      </c>
+      <c r="H62">
+        <v>2</v>
+      </c>
+      <c r="I62">
+        <v>3</v>
+      </c>
+      <c r="J62">
+        <v>2</v>
+      </c>
+      <c r="K62">
+        <v>2</v>
+      </c>
+      <c r="L62">
+        <v>7</v>
+      </c>
+      <c r="M62">
+        <v>6</v>
+      </c>
+      <c r="N62">
+        <v>2</v>
+      </c>
+      <c r="O62">
+        <v>3</v>
+      </c>
+      <c r="P62">
+        <v>3</v>
+      </c>
+      <c r="Q62">
+        <v>6</v>
+      </c>
+      <c r="R62">
+        <v>3</v>
+      </c>
+      <c r="S62">
+        <v>3</v>
+      </c>
+      <c r="T62">
+        <v>7</v>
+      </c>
+      <c r="U62">
+        <v>5</v>
+      </c>
+      <c r="V62">
+        <v>3</v>
+      </c>
+      <c r="W62">
+        <v>5</v>
+      </c>
+      <c r="X62">
+        <v>3</v>
+      </c>
+      <c r="Y62">
+        <v>3</v>
+      </c>
+      <c r="Z62">
+        <v>3</v>
+      </c>
+      <c r="AA62">
+        <v>2</v>
+      </c>
+      <c r="AB62">
+        <v>0</v>
+      </c>
+      <c r="AC62">
+        <v>6</v>
+      </c>
+      <c r="AD62">
+        <v>2</v>
+      </c>
+      <c r="AE62">
+        <v>1</v>
+      </c>
+      <c r="AF62">
+        <v>0</v>
+      </c>
+      <c r="AG62">
+        <v>2</v>
+      </c>
+      <c r="AH62">
+        <v>4</v>
+      </c>
+      <c r="AI62">
+        <v>3</v>
+      </c>
+      <c r="AJ62">
+        <v>2</v>
+      </c>
+      <c r="AK62">
+        <v>5</v>
+      </c>
+      <c r="AL62">
+        <v>1</v>
+      </c>
+      <c r="AM62">
+        <v>6</v>
+      </c>
+      <c r="AN62">
+        <v>2</v>
+      </c>
+      <c r="AO62">
+        <v>0</v>
+      </c>
+      <c r="AP62">
+        <v>2</v>
+      </c>
+      <c r="AQ62">
+        <v>1</v>
+      </c>
+      <c r="AR62">
+        <v>0</v>
+      </c>
+      <c r="AS62">
+        <v>4</v>
+      </c>
+      <c r="AT62">
+        <v>8</v>
+      </c>
+      <c r="AU62">
+        <v>3</v>
+      </c>
+      <c r="AV62">
+        <v>5</v>
+      </c>
+      <c r="AW62">
+        <v>4</v>
+      </c>
+      <c r="AX62">
+        <v>8</v>
+      </c>
+      <c r="AY62">
+        <v>2</v>
+      </c>
+      <c r="AZ62">
+        <v>1</v>
+      </c>
+      <c r="BA62">
+        <v>3</v>
+      </c>
+      <c r="BB62">
+        <v>3</v>
+      </c>
+      <c r="BC62">
+        <v>6</v>
+      </c>
+      <c r="BD62">
+        <v>5</v>
+      </c>
+      <c r="BE62">
+        <v>0</v>
+      </c>
+      <c r="BF62">
+        <v>0</v>
+      </c>
+      <c r="BG62">
+        <v>3</v>
+      </c>
+      <c r="BH62">
+        <v>1</v>
+      </c>
+      <c r="BI62">
+        <v>9</v>
+      </c>
+      <c r="BJ62">
+        <v>5</v>
+      </c>
+      <c r="BK62">
+        <v>2</v>
+      </c>
+      <c r="BL62">
+        <v>3</v>
+      </c>
+      <c r="BM62">
+        <v>2</v>
+      </c>
+      <c r="BN62">
+        <v>2</v>
+      </c>
+      <c r="BO62">
+        <v>6</v>
+      </c>
+      <c r="BP62">
+        <v>6</v>
+      </c>
+      <c r="BQ62">
+        <v>4</v>
+      </c>
+      <c r="BR62">
+        <v>3</v>
+      </c>
+      <c r="BS62">
+        <v>2</v>
+      </c>
+      <c r="BT62">
+        <v>2</v>
+      </c>
+      <c r="BU62">
+        <v>0</v>
+      </c>
+      <c r="BV62">
+        <v>2</v>
+      </c>
+      <c r="BW62">
+        <v>3</v>
+      </c>
+      <c r="BX62">
+        <v>2</v>
+      </c>
+      <c r="BY62">
+        <v>3</v>
+      </c>
+      <c r="BZ62">
+        <v>0</v>
+      </c>
+      <c r="CA62">
+        <v>2</v>
+      </c>
+      <c r="CB62">
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:80" x14ac:dyDescent="0.25">
@@ -14090,28 +15678,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
adding Latin names for pg. 180
</commit_message>
<xml_diff>
--- a/Lovejoy data table_Frequency of capture.xlsx
+++ b/Lovejoy data table_Frequency of capture.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
   <si>
     <t>Bird Species</t>
   </si>
@@ -125,6 +125,66 @@
   </si>
   <si>
     <t>Coccyzus euleri</t>
+  </si>
+  <si>
+    <t>Phaethornis superciliosus</t>
+  </si>
+  <si>
+    <t>Pipra fasciicauda</t>
+  </si>
+  <si>
+    <t>Turdus fumigatus</t>
+  </si>
+  <si>
+    <t>Basileuterus rivularis</t>
+  </si>
+  <si>
+    <t>Phaethornis ruber</t>
+  </si>
+  <si>
+    <t>Chloroceryle inda</t>
+  </si>
+  <si>
+    <t>Xiphorphynchus guttatus</t>
+  </si>
+  <si>
+    <t>Philydor pyrrhodes</t>
+  </si>
+  <si>
+    <t>Thamnophilus aethiops</t>
+  </si>
+  <si>
+    <t>Pipra iris</t>
+  </si>
+  <si>
+    <t>Notharctus tectus</t>
+  </si>
+  <si>
+    <t>Pteroglossus aracari</t>
+  </si>
+  <si>
+    <t>Cotinga cayana</t>
+  </si>
+  <si>
+    <t>Cyanerpes cyaneus</t>
+  </si>
+  <si>
+    <t>Euphonia violacea</t>
+  </si>
+  <si>
+    <t>Nyctidromus albicollis</t>
+  </si>
+  <si>
+    <t>Piaya minuta</t>
+  </si>
+  <si>
+    <t>Trogon violaceus</t>
+  </si>
+  <si>
+    <t>Pteroglossus bitorquatus</t>
+  </si>
+  <si>
+    <t>Veniliornis affinis</t>
   </si>
 </sst>
 </file>
@@ -474,11 +534,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CB64"/>
+  <dimension ref="A1:CC64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H78" sqref="H78"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10651,6 +10711,9 @@
       <c r="A43">
         <v>331</v>
       </c>
+      <c r="B43" t="s">
+        <v>37</v>
+      </c>
       <c r="C43">
         <v>217</v>
       </c>
@@ -10890,6 +10953,9 @@
       <c r="A44">
         <v>336</v>
       </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
       <c r="C44">
         <v>1</v>
       </c>
@@ -11129,6 +11195,9 @@
       <c r="A45">
         <v>337</v>
       </c>
+      <c r="B45" t="s">
+        <v>48</v>
+      </c>
       <c r="C45">
         <v>0</v>
       </c>
@@ -11368,6 +11437,9 @@
       <c r="A46">
         <v>343</v>
       </c>
+      <c r="B46" t="s">
+        <v>49</v>
+      </c>
       <c r="C46">
         <v>0</v>
       </c>
@@ -11607,6 +11679,9 @@
       <c r="A47">
         <v>344</v>
       </c>
+      <c r="B47" t="s">
+        <v>38</v>
+      </c>
       <c r="C47">
         <v>41</v>
       </c>
@@ -11846,6 +11921,9 @@
       <c r="A48">
         <v>350</v>
       </c>
+      <c r="B48" t="s">
+        <v>39</v>
+      </c>
       <c r="C48">
         <v>162</v>
       </c>
@@ -12081,10 +12159,13 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>351</v>
       </c>
+      <c r="B49" t="s">
+        <v>7</v>
+      </c>
       <c r="C49">
         <v>7</v>
       </c>
@@ -12320,10 +12401,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>355</v>
       </c>
+      <c r="B50" t="s">
+        <v>50</v>
+      </c>
       <c r="C50">
         <v>2</v>
       </c>
@@ -12559,10 +12643,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>356</v>
       </c>
+      <c r="B51" t="s">
+        <v>40</v>
+      </c>
       <c r="C51">
         <v>28</v>
       </c>
@@ -12798,10 +12885,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>359</v>
       </c>
+      <c r="B52" t="s">
+        <v>51</v>
+      </c>
       <c r="C52">
         <v>0</v>
       </c>
@@ -13037,10 +13127,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>425</v>
       </c>
+      <c r="B53" t="s">
+        <v>53</v>
+      </c>
       <c r="C53">
         <v>6</v>
       </c>
@@ -13276,10 +13369,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>429</v>
       </c>
+      <c r="B54" t="s">
+        <v>52</v>
+      </c>
       <c r="C54">
         <v>1</v>
       </c>
@@ -13515,10 +13611,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>431</v>
       </c>
+      <c r="B55" t="s">
+        <v>41</v>
+      </c>
       <c r="C55">
         <v>22</v>
       </c>
@@ -13754,10 +13853,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>432</v>
       </c>
+      <c r="B56" t="s">
+        <v>54</v>
+      </c>
       <c r="C56">
         <v>1</v>
       </c>
@@ -13993,10 +14095,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>433</v>
       </c>
+      <c r="B57" t="s">
+        <v>42</v>
+      </c>
       <c r="C57">
         <v>189</v>
       </c>
@@ -14232,10 +14337,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>437</v>
       </c>
+      <c r="B58" t="s">
+        <v>55</v>
+      </c>
       <c r="C58">
         <v>7</v>
       </c>
@@ -14471,10 +14579,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>438</v>
       </c>
+      <c r="B59" t="s">
+        <v>56</v>
+      </c>
       <c r="C59">
         <v>4</v>
       </c>
@@ -14710,10 +14821,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>439</v>
       </c>
+      <c r="B60" t="s">
+        <v>43</v>
+      </c>
       <c r="C60">
         <v>24</v>
       </c>
@@ -14949,10 +15063,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>440</v>
       </c>
+      <c r="B61" t="s">
+        <v>44</v>
+      </c>
       <c r="C61">
         <v>89</v>
       </c>
@@ -15188,10 +15305,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>441</v>
       </c>
+      <c r="B62" t="s">
+        <v>45</v>
+      </c>
       <c r="C62">
         <v>242</v>
       </c>
@@ -15427,10 +15547,13 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>444</v>
       </c>
+      <c r="B63" t="s">
+        <v>46</v>
+      </c>
       <c r="C63">
         <v>14</v>
       </c>
@@ -15666,12 +15789,250 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:80" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:81" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>448</v>
       </c>
+      <c r="B64" t="s">
+        <v>26</v>
+      </c>
       <c r="C64">
         <v>100</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>1</v>
+      </c>
+      <c r="F64">
+        <v>2</v>
+      </c>
+      <c r="G64">
+        <v>3</v>
+      </c>
+      <c r="H64">
+        <v>1</v>
+      </c>
+      <c r="I64">
+        <v>1</v>
+      </c>
+      <c r="J64">
+        <v>5</v>
+      </c>
+      <c r="K64">
+        <v>0</v>
+      </c>
+      <c r="L64">
+        <v>3</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+      <c r="N64">
+        <v>0</v>
+      </c>
+      <c r="O64">
+        <v>1</v>
+      </c>
+      <c r="P64">
+        <v>5</v>
+      </c>
+      <c r="Q64">
+        <v>2</v>
+      </c>
+      <c r="R64">
+        <v>4</v>
+      </c>
+      <c r="S64">
+        <v>0</v>
+      </c>
+      <c r="T64">
+        <v>4</v>
+      </c>
+      <c r="U64">
+        <v>4</v>
+      </c>
+      <c r="V64">
+        <v>1</v>
+      </c>
+      <c r="W64">
+        <v>5</v>
+      </c>
+      <c r="X64">
+        <v>2</v>
+      </c>
+      <c r="Y64">
+        <v>3</v>
+      </c>
+      <c r="Z64">
+        <v>1</v>
+      </c>
+      <c r="AA64">
+        <v>3</v>
+      </c>
+      <c r="AB64">
+        <v>1</v>
+      </c>
+      <c r="AC64">
+        <v>3</v>
+      </c>
+      <c r="AD64">
+        <v>2</v>
+      </c>
+      <c r="AE64">
+        <v>0</v>
+      </c>
+      <c r="AF64">
+        <v>0</v>
+      </c>
+      <c r="AG64">
+        <v>0</v>
+      </c>
+      <c r="AH64">
+        <v>0</v>
+      </c>
+      <c r="AI64">
+        <v>0</v>
+      </c>
+      <c r="AJ64">
+        <v>0</v>
+      </c>
+      <c r="AK64">
+        <v>1</v>
+      </c>
+      <c r="AL64">
+        <v>3</v>
+      </c>
+      <c r="AM64">
+        <v>4</v>
+      </c>
+      <c r="AN64">
+        <v>0</v>
+      </c>
+      <c r="AO64">
+        <v>3</v>
+      </c>
+      <c r="AP64">
+        <v>1</v>
+      </c>
+      <c r="AQ64">
+        <v>1</v>
+      </c>
+      <c r="AR64">
+        <v>0</v>
+      </c>
+      <c r="AS64">
+        <v>3</v>
+      </c>
+      <c r="AT64">
+        <v>1</v>
+      </c>
+      <c r="AU64">
+        <v>0</v>
+      </c>
+      <c r="AV64">
+        <v>0</v>
+      </c>
+      <c r="AW64">
+        <v>0</v>
+      </c>
+      <c r="AX64">
+        <v>0</v>
+      </c>
+      <c r="AY64">
+        <v>0</v>
+      </c>
+      <c r="AZ64">
+        <v>0</v>
+      </c>
+      <c r="BA64">
+        <v>0</v>
+      </c>
+      <c r="BB64">
+        <v>0</v>
+      </c>
+      <c r="BC64">
+        <v>0</v>
+      </c>
+      <c r="BD64">
+        <v>0</v>
+      </c>
+      <c r="BE64">
+        <v>0</v>
+      </c>
+      <c r="BF64">
+        <v>0</v>
+      </c>
+      <c r="BG64">
+        <v>0</v>
+      </c>
+      <c r="BH64">
+        <v>1</v>
+      </c>
+      <c r="BI64">
+        <v>2</v>
+      </c>
+      <c r="BJ64">
+        <v>5</v>
+      </c>
+      <c r="BK64">
+        <v>4</v>
+      </c>
+      <c r="BL64">
+        <v>1</v>
+      </c>
+      <c r="BM64">
+        <v>0</v>
+      </c>
+      <c r="BN64">
+        <v>1</v>
+      </c>
+      <c r="BO64">
+        <v>9</v>
+      </c>
+      <c r="BP64">
+        <v>0</v>
+      </c>
+      <c r="BQ64">
+        <v>0</v>
+      </c>
+      <c r="BR64">
+        <v>0</v>
+      </c>
+      <c r="BS64">
+        <v>0</v>
+      </c>
+      <c r="BT64">
+        <v>0</v>
+      </c>
+      <c r="BU64">
+        <v>0</v>
+      </c>
+      <c r="BV64">
+        <v>1</v>
+      </c>
+      <c r="BW64">
+        <v>0</v>
+      </c>
+      <c r="BX64">
+        <v>0</v>
+      </c>
+      <c r="BY64">
+        <v>0</v>
+      </c>
+      <c r="BZ64">
+        <v>0</v>
+      </c>
+      <c r="CA64">
+        <v>1</v>
+      </c>
+      <c r="CB64">
+        <v>0</v>
+      </c>
+      <c r="CC64">
+        <f>SUM(D64:CB64)</f>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added species ID and frequency totals for pg 181
</commit_message>
<xml_diff>
--- a/Lovejoy data table_Frequency of capture.xlsx
+++ b/Lovejoy data table_Frequency of capture.xlsx
@@ -534,11 +534,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CC64"/>
+  <dimension ref="A1:CB86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12159,7 +12159,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>351</v>
       </c>
@@ -12401,7 +12401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>355</v>
       </c>
@@ -12643,7 +12643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>356</v>
       </c>
@@ -12885,7 +12885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>359</v>
       </c>
@@ -13127,7 +13127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>425</v>
       </c>
@@ -13369,7 +13369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>429</v>
       </c>
@@ -13611,7 +13611,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>431</v>
       </c>
@@ -13853,7 +13853,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>432</v>
       </c>
@@ -14095,7 +14095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>433</v>
       </c>
@@ -14337,7 +14337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>437</v>
       </c>
@@ -14579,7 +14579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>438</v>
       </c>
@@ -14821,7 +14821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>439</v>
       </c>
@@ -15063,7 +15063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>440</v>
       </c>
@@ -15305,7 +15305,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>441</v>
       </c>
@@ -15547,7 +15547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>444</v>
       </c>
@@ -15789,7 +15789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:81" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>448</v>
       </c>
@@ -16030,9 +16030,1336 @@
       <c r="CB64">
         <v>0</v>
       </c>
-      <c r="CC64">
-        <f>SUM(D64:CB64)</f>
-        <v>99</v>
+    </row>
+    <row r="65" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>454</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>0</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+      <c r="K65">
+        <v>0</v>
+      </c>
+      <c r="L65">
+        <v>0</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+      <c r="N65">
+        <v>0</v>
+      </c>
+      <c r="O65">
+        <v>0</v>
+      </c>
+      <c r="P65">
+        <v>0</v>
+      </c>
+      <c r="Q65">
+        <v>0</v>
+      </c>
+      <c r="R65">
+        <v>0</v>
+      </c>
+      <c r="S65">
+        <v>0</v>
+      </c>
+      <c r="T65">
+        <v>0</v>
+      </c>
+      <c r="U65">
+        <v>0</v>
+      </c>
+      <c r="V65">
+        <v>0</v>
+      </c>
+      <c r="W65">
+        <v>0</v>
+      </c>
+      <c r="X65">
+        <v>0</v>
+      </c>
+      <c r="Y65">
+        <v>0</v>
+      </c>
+      <c r="Z65">
+        <v>0</v>
+      </c>
+      <c r="AA65">
+        <v>0</v>
+      </c>
+      <c r="AB65">
+        <v>0</v>
+      </c>
+      <c r="AC65">
+        <v>0</v>
+      </c>
+      <c r="AD65">
+        <v>0</v>
+      </c>
+      <c r="AE65">
+        <v>0</v>
+      </c>
+      <c r="AF65">
+        <v>0</v>
+      </c>
+      <c r="AG65">
+        <v>0</v>
+      </c>
+      <c r="AH65">
+        <v>0</v>
+      </c>
+      <c r="AI65">
+        <v>0</v>
+      </c>
+      <c r="AJ65">
+        <v>0</v>
+      </c>
+      <c r="AK65">
+        <v>0</v>
+      </c>
+      <c r="AL65">
+        <v>0</v>
+      </c>
+      <c r="AM65">
+        <v>0</v>
+      </c>
+      <c r="AN65">
+        <v>0</v>
+      </c>
+      <c r="AO65">
+        <v>0</v>
+      </c>
+      <c r="AP65">
+        <v>0</v>
+      </c>
+      <c r="AQ65">
+        <v>0</v>
+      </c>
+      <c r="AR65">
+        <v>0</v>
+      </c>
+      <c r="AS65">
+        <v>0</v>
+      </c>
+      <c r="AT65">
+        <v>0</v>
+      </c>
+      <c r="AU65">
+        <v>0</v>
+      </c>
+      <c r="AV65">
+        <v>0</v>
+      </c>
+      <c r="AW65">
+        <v>0</v>
+      </c>
+      <c r="AX65">
+        <v>0</v>
+      </c>
+      <c r="AY65">
+        <v>0</v>
+      </c>
+      <c r="AZ65">
+        <v>0</v>
+      </c>
+      <c r="BA65">
+        <v>0</v>
+      </c>
+      <c r="BB65">
+        <v>0</v>
+      </c>
+      <c r="BC65">
+        <v>0</v>
+      </c>
+      <c r="BD65">
+        <v>0</v>
+      </c>
+      <c r="BE65">
+        <v>0</v>
+      </c>
+      <c r="BF65">
+        <v>0</v>
+      </c>
+      <c r="BG65">
+        <v>0</v>
+      </c>
+      <c r="BH65">
+        <v>0</v>
+      </c>
+      <c r="BI65">
+        <v>0</v>
+      </c>
+      <c r="BJ65">
+        <v>0</v>
+      </c>
+      <c r="BK65">
+        <v>0</v>
+      </c>
+      <c r="BL65">
+        <v>0</v>
+      </c>
+      <c r="BM65">
+        <v>0</v>
+      </c>
+      <c r="BN65">
+        <v>0</v>
+      </c>
+      <c r="BO65">
+        <v>0</v>
+      </c>
+      <c r="BP65">
+        <v>0</v>
+      </c>
+      <c r="BQ65">
+        <v>0</v>
+      </c>
+      <c r="BR65">
+        <v>0</v>
+      </c>
+      <c r="BS65">
+        <v>0</v>
+      </c>
+      <c r="BT65">
+        <v>0</v>
+      </c>
+      <c r="BU65">
+        <v>0</v>
+      </c>
+      <c r="BV65">
+        <v>0</v>
+      </c>
+      <c r="BW65">
+        <v>0</v>
+      </c>
+      <c r="BX65">
+        <v>0</v>
+      </c>
+      <c r="BY65">
+        <v>0</v>
+      </c>
+      <c r="BZ65">
+        <v>0</v>
+      </c>
+      <c r="CA65">
+        <v>0</v>
+      </c>
+      <c r="CB65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>455</v>
+      </c>
+      <c r="C66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>457</v>
+      </c>
+      <c r="C67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>459</v>
+      </c>
+      <c r="C68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>501</v>
+      </c>
+      <c r="C69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>523</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>527</v>
+      </c>
+      <c r="C71">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>530</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>0</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+      <c r="K72">
+        <v>0</v>
+      </c>
+      <c r="L72">
+        <v>0</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+      <c r="N72">
+        <v>0</v>
+      </c>
+      <c r="O72">
+        <v>0</v>
+      </c>
+      <c r="P72">
+        <v>0</v>
+      </c>
+      <c r="Q72">
+        <v>0</v>
+      </c>
+      <c r="R72">
+        <v>0</v>
+      </c>
+      <c r="S72">
+        <v>0</v>
+      </c>
+      <c r="T72">
+        <v>0</v>
+      </c>
+      <c r="U72">
+        <v>0</v>
+      </c>
+      <c r="V72">
+        <v>0</v>
+      </c>
+      <c r="W72">
+        <v>0</v>
+      </c>
+      <c r="X72">
+        <v>0</v>
+      </c>
+      <c r="Y72">
+        <v>0</v>
+      </c>
+      <c r="Z72">
+        <v>0</v>
+      </c>
+      <c r="AA72">
+        <v>0</v>
+      </c>
+      <c r="AB72">
+        <v>0</v>
+      </c>
+      <c r="AC72">
+        <v>0</v>
+      </c>
+      <c r="AD72">
+        <v>0</v>
+      </c>
+      <c r="AE72">
+        <v>0</v>
+      </c>
+      <c r="AF72">
+        <v>0</v>
+      </c>
+      <c r="AG72">
+        <v>0</v>
+      </c>
+      <c r="AH72">
+        <v>0</v>
+      </c>
+      <c r="AI72">
+        <v>0</v>
+      </c>
+      <c r="AJ72">
+        <v>0</v>
+      </c>
+      <c r="AK72">
+        <v>0</v>
+      </c>
+      <c r="AL72">
+        <v>0</v>
+      </c>
+      <c r="AM72">
+        <v>0</v>
+      </c>
+      <c r="AN72">
+        <v>0</v>
+      </c>
+      <c r="AO72">
+        <v>0</v>
+      </c>
+      <c r="AP72">
+        <v>0</v>
+      </c>
+      <c r="AQ72">
+        <v>0</v>
+      </c>
+      <c r="AR72">
+        <v>0</v>
+      </c>
+      <c r="AS72">
+        <v>0</v>
+      </c>
+      <c r="AT72">
+        <v>0</v>
+      </c>
+      <c r="AU72">
+        <v>0</v>
+      </c>
+      <c r="AV72">
+        <v>0</v>
+      </c>
+      <c r="AW72">
+        <v>0</v>
+      </c>
+      <c r="AX72">
+        <v>0</v>
+      </c>
+      <c r="AY72">
+        <v>0</v>
+      </c>
+      <c r="AZ72">
+        <v>0</v>
+      </c>
+      <c r="BA72">
+        <v>0</v>
+      </c>
+      <c r="BB72">
+        <v>0</v>
+      </c>
+      <c r="BC72">
+        <v>0</v>
+      </c>
+      <c r="BD72">
+        <v>0</v>
+      </c>
+      <c r="BE72">
+        <v>0</v>
+      </c>
+      <c r="BF72">
+        <v>0</v>
+      </c>
+      <c r="BG72">
+        <v>0</v>
+      </c>
+      <c r="BH72">
+        <v>0</v>
+      </c>
+      <c r="BI72">
+        <v>0</v>
+      </c>
+      <c r="BJ72">
+        <v>0</v>
+      </c>
+      <c r="BK72">
+        <v>0</v>
+      </c>
+      <c r="BL72">
+        <v>0</v>
+      </c>
+      <c r="BM72">
+        <v>0</v>
+      </c>
+      <c r="BN72">
+        <v>0</v>
+      </c>
+      <c r="BO72">
+        <v>0</v>
+      </c>
+      <c r="BP72">
+        <v>0</v>
+      </c>
+      <c r="BQ72">
+        <v>0</v>
+      </c>
+      <c r="BR72">
+        <v>0</v>
+      </c>
+      <c r="BS72">
+        <v>0</v>
+      </c>
+      <c r="BT72">
+        <v>0</v>
+      </c>
+      <c r="BU72">
+        <v>0</v>
+      </c>
+      <c r="BV72">
+        <v>0</v>
+      </c>
+      <c r="BW72">
+        <v>0</v>
+      </c>
+      <c r="BX72">
+        <v>0</v>
+      </c>
+      <c r="BY72">
+        <v>0</v>
+      </c>
+      <c r="BZ72">
+        <v>0</v>
+      </c>
+      <c r="CA72">
+        <v>0</v>
+      </c>
+      <c r="CB72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>531</v>
+      </c>
+      <c r="C73">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="74" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>532</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>0</v>
+      </c>
+      <c r="J74">
+        <v>0</v>
+      </c>
+      <c r="K74">
+        <v>0</v>
+      </c>
+      <c r="L74">
+        <v>0</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+      <c r="N74">
+        <v>0</v>
+      </c>
+      <c r="O74">
+        <v>0</v>
+      </c>
+      <c r="P74">
+        <v>0</v>
+      </c>
+      <c r="Q74">
+        <v>0</v>
+      </c>
+      <c r="R74">
+        <v>0</v>
+      </c>
+      <c r="S74">
+        <v>0</v>
+      </c>
+      <c r="T74">
+        <v>0</v>
+      </c>
+      <c r="U74">
+        <v>0</v>
+      </c>
+      <c r="V74">
+        <v>0</v>
+      </c>
+      <c r="W74">
+        <v>0</v>
+      </c>
+      <c r="X74">
+        <v>0</v>
+      </c>
+      <c r="Y74">
+        <v>0</v>
+      </c>
+      <c r="Z74">
+        <v>0</v>
+      </c>
+      <c r="AA74">
+        <v>0</v>
+      </c>
+      <c r="AB74">
+        <v>0</v>
+      </c>
+      <c r="AC74">
+        <v>0</v>
+      </c>
+      <c r="AD74">
+        <v>0</v>
+      </c>
+      <c r="AE74">
+        <v>0</v>
+      </c>
+      <c r="AF74">
+        <v>0</v>
+      </c>
+      <c r="AG74">
+        <v>0</v>
+      </c>
+      <c r="AH74">
+        <v>0</v>
+      </c>
+      <c r="AI74">
+        <v>0</v>
+      </c>
+      <c r="AJ74">
+        <v>0</v>
+      </c>
+      <c r="AK74">
+        <v>0</v>
+      </c>
+      <c r="AL74">
+        <v>0</v>
+      </c>
+      <c r="AM74">
+        <v>0</v>
+      </c>
+      <c r="AN74">
+        <v>0</v>
+      </c>
+      <c r="AO74">
+        <v>0</v>
+      </c>
+      <c r="AP74">
+        <v>0</v>
+      </c>
+      <c r="AQ74">
+        <v>0</v>
+      </c>
+      <c r="AR74">
+        <v>0</v>
+      </c>
+      <c r="AS74">
+        <v>0</v>
+      </c>
+      <c r="AT74">
+        <v>0</v>
+      </c>
+      <c r="AU74">
+        <v>0</v>
+      </c>
+      <c r="AV74">
+        <v>0</v>
+      </c>
+      <c r="AW74">
+        <v>0</v>
+      </c>
+      <c r="AX74">
+        <v>0</v>
+      </c>
+      <c r="AY74">
+        <v>0</v>
+      </c>
+      <c r="AZ74">
+        <v>0</v>
+      </c>
+      <c r="BA74">
+        <v>0</v>
+      </c>
+      <c r="BB74">
+        <v>0</v>
+      </c>
+      <c r="BC74">
+        <v>0</v>
+      </c>
+      <c r="BD74">
+        <v>0</v>
+      </c>
+      <c r="BE74">
+        <v>0</v>
+      </c>
+      <c r="BF74">
+        <v>0</v>
+      </c>
+      <c r="BG74">
+        <v>0</v>
+      </c>
+      <c r="BH74">
+        <v>0</v>
+      </c>
+      <c r="BI74">
+        <v>0</v>
+      </c>
+      <c r="BJ74">
+        <v>0</v>
+      </c>
+      <c r="BK74">
+        <v>0</v>
+      </c>
+      <c r="BL74">
+        <v>0</v>
+      </c>
+      <c r="BM74">
+        <v>0</v>
+      </c>
+      <c r="BN74">
+        <v>0</v>
+      </c>
+      <c r="BO74">
+        <v>0</v>
+      </c>
+      <c r="BP74">
+        <v>0</v>
+      </c>
+      <c r="BQ74">
+        <v>0</v>
+      </c>
+      <c r="BR74">
+        <v>0</v>
+      </c>
+      <c r="BS74">
+        <v>0</v>
+      </c>
+      <c r="BT74">
+        <v>0</v>
+      </c>
+      <c r="BU74">
+        <v>0</v>
+      </c>
+      <c r="BV74">
+        <v>0</v>
+      </c>
+      <c r="BW74">
+        <v>0</v>
+      </c>
+      <c r="BX74">
+        <v>0</v>
+      </c>
+      <c r="BY74">
+        <v>0</v>
+      </c>
+      <c r="BZ74">
+        <v>0</v>
+      </c>
+      <c r="CA74">
+        <v>0</v>
+      </c>
+      <c r="CB74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>533</v>
+      </c>
+      <c r="C75">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="76" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>536</v>
+      </c>
+      <c r="C76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>537</v>
+      </c>
+      <c r="C77">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>538</v>
+      </c>
+      <c r="C78">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>539</v>
+      </c>
+      <c r="C79">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="80" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>540</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>0</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+      <c r="I80">
+        <v>0</v>
+      </c>
+      <c r="J80">
+        <v>0</v>
+      </c>
+      <c r="K80">
+        <v>0</v>
+      </c>
+      <c r="L80">
+        <v>0</v>
+      </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+      <c r="N80">
+        <v>0</v>
+      </c>
+      <c r="O80">
+        <v>0</v>
+      </c>
+      <c r="P80">
+        <v>0</v>
+      </c>
+      <c r="Q80">
+        <v>0</v>
+      </c>
+      <c r="R80">
+        <v>0</v>
+      </c>
+      <c r="S80">
+        <v>0</v>
+      </c>
+      <c r="T80">
+        <v>0</v>
+      </c>
+      <c r="U80">
+        <v>0</v>
+      </c>
+      <c r="V80">
+        <v>0</v>
+      </c>
+      <c r="W80">
+        <v>0</v>
+      </c>
+      <c r="X80">
+        <v>0</v>
+      </c>
+      <c r="Y80">
+        <v>0</v>
+      </c>
+      <c r="Z80">
+        <v>0</v>
+      </c>
+      <c r="AA80">
+        <v>0</v>
+      </c>
+      <c r="AB80">
+        <v>0</v>
+      </c>
+      <c r="AC80">
+        <v>0</v>
+      </c>
+      <c r="AD80">
+        <v>0</v>
+      </c>
+      <c r="AE80">
+        <v>0</v>
+      </c>
+      <c r="AF80">
+        <v>0</v>
+      </c>
+      <c r="AG80">
+        <v>0</v>
+      </c>
+      <c r="AH80">
+        <v>0</v>
+      </c>
+      <c r="AI80">
+        <v>0</v>
+      </c>
+      <c r="AJ80">
+        <v>0</v>
+      </c>
+      <c r="AK80">
+        <v>0</v>
+      </c>
+      <c r="AL80">
+        <v>0</v>
+      </c>
+      <c r="AM80">
+        <v>0</v>
+      </c>
+      <c r="AN80">
+        <v>0</v>
+      </c>
+      <c r="AO80">
+        <v>0</v>
+      </c>
+      <c r="AP80">
+        <v>0</v>
+      </c>
+      <c r="AQ80">
+        <v>0</v>
+      </c>
+      <c r="AR80">
+        <v>0</v>
+      </c>
+      <c r="AS80">
+        <v>0</v>
+      </c>
+      <c r="AT80">
+        <v>0</v>
+      </c>
+      <c r="AU80">
+        <v>0</v>
+      </c>
+      <c r="AV80">
+        <v>0</v>
+      </c>
+      <c r="AW80">
+        <v>0</v>
+      </c>
+      <c r="AX80">
+        <v>0</v>
+      </c>
+      <c r="AY80">
+        <v>0</v>
+      </c>
+      <c r="AZ80">
+        <v>0</v>
+      </c>
+      <c r="BA80">
+        <v>0</v>
+      </c>
+      <c r="BB80">
+        <v>0</v>
+      </c>
+      <c r="BC80">
+        <v>0</v>
+      </c>
+      <c r="BD80">
+        <v>0</v>
+      </c>
+      <c r="BE80">
+        <v>0</v>
+      </c>
+      <c r="BF80">
+        <v>0</v>
+      </c>
+      <c r="BG80">
+        <v>0</v>
+      </c>
+      <c r="BH80">
+        <v>0</v>
+      </c>
+      <c r="BI80">
+        <v>0</v>
+      </c>
+      <c r="BJ80">
+        <v>0</v>
+      </c>
+      <c r="BK80">
+        <v>0</v>
+      </c>
+      <c r="BL80">
+        <v>0</v>
+      </c>
+      <c r="BM80">
+        <v>0</v>
+      </c>
+      <c r="BN80">
+        <v>0</v>
+      </c>
+      <c r="BO80">
+        <v>0</v>
+      </c>
+      <c r="BP80">
+        <v>0</v>
+      </c>
+      <c r="BQ80">
+        <v>0</v>
+      </c>
+      <c r="BR80">
+        <v>0</v>
+      </c>
+      <c r="BS80">
+        <v>0</v>
+      </c>
+      <c r="BT80">
+        <v>0</v>
+      </c>
+      <c r="BU80">
+        <v>0</v>
+      </c>
+      <c r="BV80">
+        <v>0</v>
+      </c>
+      <c r="BW80">
+        <v>0</v>
+      </c>
+      <c r="BX80">
+        <v>0</v>
+      </c>
+      <c r="BY80">
+        <v>0</v>
+      </c>
+      <c r="BZ80">
+        <v>0</v>
+      </c>
+      <c r="CA80">
+        <v>0</v>
+      </c>
+      <c r="CB80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>541</v>
+      </c>
+      <c r="C81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>544</v>
+      </c>
+      <c r="C82">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="83" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>550</v>
+      </c>
+      <c r="C83">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>557</v>
+      </c>
+      <c r="C84">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="85" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>623</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>0</v>
+      </c>
+      <c r="K85">
+        <v>0</v>
+      </c>
+      <c r="L85">
+        <v>0</v>
+      </c>
+      <c r="M85">
+        <v>0</v>
+      </c>
+      <c r="N85">
+        <v>0</v>
+      </c>
+      <c r="O85">
+        <v>0</v>
+      </c>
+      <c r="P85">
+        <v>0</v>
+      </c>
+      <c r="Q85">
+        <v>0</v>
+      </c>
+      <c r="R85">
+        <v>0</v>
+      </c>
+      <c r="S85">
+        <v>0</v>
+      </c>
+      <c r="T85">
+        <v>0</v>
+      </c>
+      <c r="U85">
+        <v>0</v>
+      </c>
+      <c r="V85">
+        <v>0</v>
+      </c>
+      <c r="W85">
+        <v>0</v>
+      </c>
+      <c r="X85">
+        <v>0</v>
+      </c>
+      <c r="Y85">
+        <v>0</v>
+      </c>
+      <c r="Z85">
+        <v>0</v>
+      </c>
+      <c r="AA85">
+        <v>0</v>
+      </c>
+      <c r="AB85">
+        <v>0</v>
+      </c>
+      <c r="AC85">
+        <v>0</v>
+      </c>
+      <c r="AD85">
+        <v>0</v>
+      </c>
+      <c r="AE85">
+        <v>0</v>
+      </c>
+      <c r="AF85">
+        <v>0</v>
+      </c>
+      <c r="AG85">
+        <v>0</v>
+      </c>
+      <c r="AH85">
+        <v>0</v>
+      </c>
+      <c r="AI85">
+        <v>0</v>
+      </c>
+      <c r="AJ85">
+        <v>0</v>
+      </c>
+      <c r="AK85">
+        <v>0</v>
+      </c>
+      <c r="AL85">
+        <v>0</v>
+      </c>
+      <c r="AM85">
+        <v>0</v>
+      </c>
+      <c r="AN85">
+        <v>0</v>
+      </c>
+      <c r="AO85">
+        <v>0</v>
+      </c>
+      <c r="AP85">
+        <v>0</v>
+      </c>
+      <c r="AQ85">
+        <v>0</v>
+      </c>
+      <c r="AR85">
+        <v>0</v>
+      </c>
+      <c r="AS85">
+        <v>0</v>
+      </c>
+      <c r="AT85">
+        <v>0</v>
+      </c>
+      <c r="AU85">
+        <v>0</v>
+      </c>
+      <c r="AV85">
+        <v>0</v>
+      </c>
+      <c r="AW85">
+        <v>0</v>
+      </c>
+      <c r="AX85">
+        <v>0</v>
+      </c>
+      <c r="AY85">
+        <v>0</v>
+      </c>
+      <c r="AZ85">
+        <v>0</v>
+      </c>
+      <c r="BA85">
+        <v>0</v>
+      </c>
+      <c r="BB85">
+        <v>0</v>
+      </c>
+      <c r="BC85">
+        <v>0</v>
+      </c>
+      <c r="BD85">
+        <v>0</v>
+      </c>
+      <c r="BE85">
+        <v>0</v>
+      </c>
+      <c r="BF85">
+        <v>0</v>
+      </c>
+      <c r="BG85">
+        <v>0</v>
+      </c>
+      <c r="BH85">
+        <v>0</v>
+      </c>
+      <c r="BI85">
+        <v>0</v>
+      </c>
+      <c r="BJ85">
+        <v>0</v>
+      </c>
+      <c r="BK85">
+        <v>0</v>
+      </c>
+      <c r="BL85">
+        <v>0</v>
+      </c>
+      <c r="BM85">
+        <v>0</v>
+      </c>
+      <c r="BN85">
+        <v>0</v>
+      </c>
+      <c r="BO85">
+        <v>0</v>
+      </c>
+      <c r="BP85">
+        <v>0</v>
+      </c>
+      <c r="BQ85">
+        <v>0</v>
+      </c>
+      <c r="BR85">
+        <v>0</v>
+      </c>
+      <c r="BS85">
+        <v>0</v>
+      </c>
+      <c r="BT85">
+        <v>0</v>
+      </c>
+      <c r="BU85">
+        <v>0</v>
+      </c>
+      <c r="BV85">
+        <v>0</v>
+      </c>
+      <c r="BW85">
+        <v>0</v>
+      </c>
+      <c r="BX85">
+        <v>0</v>
+      </c>
+      <c r="BY85">
+        <v>0</v>
+      </c>
+      <c r="BZ85">
+        <v>0</v>
+      </c>
+      <c r="CA85">
+        <v>0</v>
+      </c>
+      <c r="CB85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:80" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>629</v>
+      </c>
+      <c r="C86">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed entering data for pg. 181
</commit_message>
<xml_diff>
--- a/Lovejoy data table_Frequency of capture.xlsx
+++ b/Lovejoy data table_Frequency of capture.xlsx
@@ -536,9 +536,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CB86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E92" sqref="E92"/>
+    <sheetView tabSelected="1" topLeftCell="BK1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="CC84" sqref="CC84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17472,6 +17472,237 @@
       <c r="C71">
         <v>5</v>
       </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>0</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71">
+        <v>0</v>
+      </c>
+      <c r="J71">
+        <v>0</v>
+      </c>
+      <c r="K71">
+        <v>2</v>
+      </c>
+      <c r="L71">
+        <v>0</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+      <c r="N71">
+        <v>0</v>
+      </c>
+      <c r="O71">
+        <v>0</v>
+      </c>
+      <c r="P71">
+        <v>0</v>
+      </c>
+      <c r="Q71">
+        <v>0</v>
+      </c>
+      <c r="R71">
+        <v>0</v>
+      </c>
+      <c r="S71">
+        <v>0</v>
+      </c>
+      <c r="T71">
+        <v>0</v>
+      </c>
+      <c r="U71">
+        <v>0</v>
+      </c>
+      <c r="V71">
+        <v>0</v>
+      </c>
+      <c r="W71">
+        <v>0</v>
+      </c>
+      <c r="X71">
+        <v>0</v>
+      </c>
+      <c r="Y71">
+        <v>0</v>
+      </c>
+      <c r="Z71">
+        <v>0</v>
+      </c>
+      <c r="AA71">
+        <v>0</v>
+      </c>
+      <c r="AB71">
+        <v>0</v>
+      </c>
+      <c r="AC71">
+        <v>1</v>
+      </c>
+      <c r="AD71">
+        <v>0</v>
+      </c>
+      <c r="AE71">
+        <v>0</v>
+      </c>
+      <c r="AF71">
+        <v>0</v>
+      </c>
+      <c r="AG71">
+        <v>0</v>
+      </c>
+      <c r="AH71">
+        <v>0</v>
+      </c>
+      <c r="AI71">
+        <v>0</v>
+      </c>
+      <c r="AJ71">
+        <v>1</v>
+      </c>
+      <c r="AK71">
+        <v>0</v>
+      </c>
+      <c r="AL71">
+        <v>0</v>
+      </c>
+      <c r="AM71">
+        <v>0</v>
+      </c>
+      <c r="AN71">
+        <v>0</v>
+      </c>
+      <c r="AO71">
+        <v>0</v>
+      </c>
+      <c r="AP71">
+        <v>0</v>
+      </c>
+      <c r="AQ71">
+        <v>0</v>
+      </c>
+      <c r="AR71">
+        <v>0</v>
+      </c>
+      <c r="AS71">
+        <v>0</v>
+      </c>
+      <c r="AT71">
+        <v>1</v>
+      </c>
+      <c r="AU71">
+        <v>0</v>
+      </c>
+      <c r="AV71">
+        <v>0</v>
+      </c>
+      <c r="AW71">
+        <v>0</v>
+      </c>
+      <c r="AX71">
+        <v>0</v>
+      </c>
+      <c r="AY71">
+        <v>0</v>
+      </c>
+      <c r="AZ71">
+        <v>0</v>
+      </c>
+      <c r="BA71">
+        <v>0</v>
+      </c>
+      <c r="BB71">
+        <v>0</v>
+      </c>
+      <c r="BC71">
+        <v>0</v>
+      </c>
+      <c r="BD71">
+        <v>0</v>
+      </c>
+      <c r="BE71">
+        <v>0</v>
+      </c>
+      <c r="BF71">
+        <v>0</v>
+      </c>
+      <c r="BG71">
+        <v>0</v>
+      </c>
+      <c r="BH71">
+        <v>0</v>
+      </c>
+      <c r="BI71">
+        <v>0</v>
+      </c>
+      <c r="BJ71">
+        <v>0</v>
+      </c>
+      <c r="BK71">
+        <v>0</v>
+      </c>
+      <c r="BL71">
+        <v>0</v>
+      </c>
+      <c r="BM71">
+        <v>0</v>
+      </c>
+      <c r="BN71">
+        <v>0</v>
+      </c>
+      <c r="BO71">
+        <v>0</v>
+      </c>
+      <c r="BP71">
+        <v>0</v>
+      </c>
+      <c r="BQ71">
+        <v>0</v>
+      </c>
+      <c r="BR71">
+        <v>0</v>
+      </c>
+      <c r="BS71">
+        <v>0</v>
+      </c>
+      <c r="BT71">
+        <v>0</v>
+      </c>
+      <c r="BU71">
+        <v>0</v>
+      </c>
+      <c r="BV71">
+        <v>0</v>
+      </c>
+      <c r="BW71">
+        <v>0</v>
+      </c>
+      <c r="BX71">
+        <v>0</v>
+      </c>
+      <c r="BY71">
+        <v>0</v>
+      </c>
+      <c r="BZ71">
+        <v>0</v>
+      </c>
+      <c r="CA71">
+        <v>0</v>
+      </c>
+      <c r="CB71">
+        <v>0</v>
+      </c>
     </row>
     <row r="72" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A72">
@@ -17719,6 +17950,237 @@
       <c r="C73">
         <v>110</v>
       </c>
+      <c r="D73">
+        <v>3</v>
+      </c>
+      <c r="E73">
+        <v>2</v>
+      </c>
+      <c r="F73">
+        <v>3</v>
+      </c>
+      <c r="G73">
+        <v>0</v>
+      </c>
+      <c r="H73">
+        <v>1</v>
+      </c>
+      <c r="I73">
+        <v>0</v>
+      </c>
+      <c r="J73">
+        <v>5</v>
+      </c>
+      <c r="K73">
+        <v>0</v>
+      </c>
+      <c r="L73">
+        <v>1</v>
+      </c>
+      <c r="M73">
+        <v>2</v>
+      </c>
+      <c r="N73">
+        <v>0</v>
+      </c>
+      <c r="O73">
+        <v>1</v>
+      </c>
+      <c r="P73">
+        <v>1</v>
+      </c>
+      <c r="Q73">
+        <v>1</v>
+      </c>
+      <c r="R73">
+        <v>1</v>
+      </c>
+      <c r="S73">
+        <v>3</v>
+      </c>
+      <c r="T73">
+        <v>2</v>
+      </c>
+      <c r="U73">
+        <v>0</v>
+      </c>
+      <c r="V73">
+        <v>2</v>
+      </c>
+      <c r="W73">
+        <v>0</v>
+      </c>
+      <c r="X73">
+        <v>3</v>
+      </c>
+      <c r="Y73">
+        <v>1</v>
+      </c>
+      <c r="Z73">
+        <v>2</v>
+      </c>
+      <c r="AA73">
+        <v>1</v>
+      </c>
+      <c r="AB73">
+        <v>2</v>
+      </c>
+      <c r="AC73">
+        <v>1</v>
+      </c>
+      <c r="AD73">
+        <v>3</v>
+      </c>
+      <c r="AE73">
+        <v>7</v>
+      </c>
+      <c r="AF73">
+        <v>3</v>
+      </c>
+      <c r="AG73">
+        <v>0</v>
+      </c>
+      <c r="AH73">
+        <v>5</v>
+      </c>
+      <c r="AI73">
+        <v>4</v>
+      </c>
+      <c r="AJ73">
+        <v>0</v>
+      </c>
+      <c r="AK73">
+        <v>0</v>
+      </c>
+      <c r="AL73">
+        <v>0</v>
+      </c>
+      <c r="AM73">
+        <v>3</v>
+      </c>
+      <c r="AN73">
+        <v>3</v>
+      </c>
+      <c r="AO73">
+        <v>3</v>
+      </c>
+      <c r="AP73">
+        <v>0</v>
+      </c>
+      <c r="AQ73">
+        <v>1</v>
+      </c>
+      <c r="AR73">
+        <v>4</v>
+      </c>
+      <c r="AS73">
+        <v>1</v>
+      </c>
+      <c r="AT73">
+        <v>0</v>
+      </c>
+      <c r="AU73">
+        <v>1</v>
+      </c>
+      <c r="AV73">
+        <v>1</v>
+      </c>
+      <c r="AW73">
+        <v>1</v>
+      </c>
+      <c r="AX73">
+        <v>2</v>
+      </c>
+      <c r="AY73">
+        <v>1</v>
+      </c>
+      <c r="AZ73">
+        <v>0</v>
+      </c>
+      <c r="BA73">
+        <v>0</v>
+      </c>
+      <c r="BB73">
+        <v>2</v>
+      </c>
+      <c r="BC73">
+        <v>5</v>
+      </c>
+      <c r="BD73">
+        <v>0</v>
+      </c>
+      <c r="BE73">
+        <v>0</v>
+      </c>
+      <c r="BF73">
+        <v>0</v>
+      </c>
+      <c r="BG73">
+        <v>0</v>
+      </c>
+      <c r="BH73">
+        <v>0</v>
+      </c>
+      <c r="BI73">
+        <v>0</v>
+      </c>
+      <c r="BJ73">
+        <v>0</v>
+      </c>
+      <c r="BK73">
+        <v>0</v>
+      </c>
+      <c r="BL73">
+        <v>0</v>
+      </c>
+      <c r="BM73">
+        <v>0</v>
+      </c>
+      <c r="BN73">
+        <v>0</v>
+      </c>
+      <c r="BO73">
+        <v>0</v>
+      </c>
+      <c r="BP73">
+        <v>3</v>
+      </c>
+      <c r="BQ73">
+        <v>2</v>
+      </c>
+      <c r="BR73">
+        <v>2</v>
+      </c>
+      <c r="BS73">
+        <v>2</v>
+      </c>
+      <c r="BT73">
+        <v>2</v>
+      </c>
+      <c r="BU73">
+        <v>3</v>
+      </c>
+      <c r="BV73">
+        <v>0</v>
+      </c>
+      <c r="BW73">
+        <v>3</v>
+      </c>
+      <c r="BX73">
+        <v>1</v>
+      </c>
+      <c r="BY73">
+        <v>1</v>
+      </c>
+      <c r="BZ73">
+        <v>3</v>
+      </c>
+      <c r="CA73">
+        <v>0</v>
+      </c>
+      <c r="CB73">
+        <v>0</v>
+      </c>
     </row>
     <row r="74" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A74">
@@ -17966,6 +18428,237 @@
       <c r="C75">
         <v>185</v>
       </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <v>0</v>
+      </c>
+      <c r="J75">
+        <v>1</v>
+      </c>
+      <c r="K75">
+        <v>0</v>
+      </c>
+      <c r="L75">
+        <v>1</v>
+      </c>
+      <c r="M75">
+        <v>1</v>
+      </c>
+      <c r="N75">
+        <v>1</v>
+      </c>
+      <c r="O75">
+        <v>0</v>
+      </c>
+      <c r="P75">
+        <v>0</v>
+      </c>
+      <c r="Q75">
+        <v>0</v>
+      </c>
+      <c r="R75">
+        <v>0</v>
+      </c>
+      <c r="S75">
+        <v>1</v>
+      </c>
+      <c r="T75">
+        <v>0</v>
+      </c>
+      <c r="U75">
+        <v>1</v>
+      </c>
+      <c r="V75">
+        <v>0</v>
+      </c>
+      <c r="W75">
+        <v>1</v>
+      </c>
+      <c r="X75">
+        <v>2</v>
+      </c>
+      <c r="Y75">
+        <v>1</v>
+      </c>
+      <c r="Z75">
+        <v>2</v>
+      </c>
+      <c r="AA75">
+        <v>2</v>
+      </c>
+      <c r="AB75">
+        <v>4</v>
+      </c>
+      <c r="AC75">
+        <v>3</v>
+      </c>
+      <c r="AD75">
+        <v>4</v>
+      </c>
+      <c r="AE75">
+        <v>5</v>
+      </c>
+      <c r="AF75">
+        <v>1</v>
+      </c>
+      <c r="AG75">
+        <v>4</v>
+      </c>
+      <c r="AH75">
+        <v>0</v>
+      </c>
+      <c r="AI75">
+        <v>2</v>
+      </c>
+      <c r="AJ75">
+        <v>1</v>
+      </c>
+      <c r="AK75">
+        <v>0</v>
+      </c>
+      <c r="AL75">
+        <v>0</v>
+      </c>
+      <c r="AM75">
+        <v>0</v>
+      </c>
+      <c r="AN75">
+        <v>1</v>
+      </c>
+      <c r="AO75">
+        <v>0</v>
+      </c>
+      <c r="AP75">
+        <v>1</v>
+      </c>
+      <c r="AQ75">
+        <v>2</v>
+      </c>
+      <c r="AR75">
+        <v>4</v>
+      </c>
+      <c r="AS75">
+        <v>0</v>
+      </c>
+      <c r="AT75">
+        <v>0</v>
+      </c>
+      <c r="AU75">
+        <v>13</v>
+      </c>
+      <c r="AV75">
+        <v>7</v>
+      </c>
+      <c r="AW75">
+        <v>2</v>
+      </c>
+      <c r="AX75">
+        <v>0</v>
+      </c>
+      <c r="AY75">
+        <v>11</v>
+      </c>
+      <c r="AZ75">
+        <v>12</v>
+      </c>
+      <c r="BA75">
+        <v>6</v>
+      </c>
+      <c r="BB75">
+        <v>10</v>
+      </c>
+      <c r="BC75">
+        <v>2</v>
+      </c>
+      <c r="BD75">
+        <v>7</v>
+      </c>
+      <c r="BE75">
+        <v>3</v>
+      </c>
+      <c r="BF75">
+        <v>0</v>
+      </c>
+      <c r="BG75">
+        <v>0</v>
+      </c>
+      <c r="BH75">
+        <v>1</v>
+      </c>
+      <c r="BI75">
+        <v>0</v>
+      </c>
+      <c r="BJ75">
+        <v>0</v>
+      </c>
+      <c r="BK75">
+        <v>1</v>
+      </c>
+      <c r="BL75">
+        <v>0</v>
+      </c>
+      <c r="BM75">
+        <v>0</v>
+      </c>
+      <c r="BN75">
+        <v>2</v>
+      </c>
+      <c r="BO75">
+        <v>1</v>
+      </c>
+      <c r="BP75">
+        <v>6</v>
+      </c>
+      <c r="BQ75">
+        <v>3</v>
+      </c>
+      <c r="BR75">
+        <v>3</v>
+      </c>
+      <c r="BS75">
+        <v>4</v>
+      </c>
+      <c r="BT75">
+        <v>4</v>
+      </c>
+      <c r="BU75">
+        <v>6</v>
+      </c>
+      <c r="BV75">
+        <v>5</v>
+      </c>
+      <c r="BW75">
+        <v>5</v>
+      </c>
+      <c r="BX75">
+        <v>3</v>
+      </c>
+      <c r="BY75">
+        <v>2</v>
+      </c>
+      <c r="BZ75">
+        <v>7</v>
+      </c>
+      <c r="CA75">
+        <v>11</v>
+      </c>
+      <c r="CB75">
+        <v>0</v>
+      </c>
     </row>
     <row r="76" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A76">
@@ -18452,6 +19145,234 @@
       <c r="C78">
         <v>25</v>
       </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+      <c r="F78">
+        <v>1</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>1</v>
+      </c>
+      <c r="I78">
+        <v>1</v>
+      </c>
+      <c r="J78">
+        <v>0</v>
+      </c>
+      <c r="K78">
+        <v>0</v>
+      </c>
+      <c r="L78">
+        <v>0</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+      <c r="N78">
+        <v>0</v>
+      </c>
+      <c r="O78">
+        <v>0</v>
+      </c>
+      <c r="P78">
+        <v>0</v>
+      </c>
+      <c r="Q78">
+        <v>0</v>
+      </c>
+      <c r="R78">
+        <v>0</v>
+      </c>
+      <c r="S78">
+        <v>0</v>
+      </c>
+      <c r="T78">
+        <v>0</v>
+      </c>
+      <c r="U78">
+        <v>0</v>
+      </c>
+      <c r="V78">
+        <v>0</v>
+      </c>
+      <c r="W78">
+        <v>2</v>
+      </c>
+      <c r="X78">
+        <v>0</v>
+      </c>
+      <c r="Y78">
+        <v>0</v>
+      </c>
+      <c r="Z78">
+        <v>1</v>
+      </c>
+      <c r="AA78">
+        <v>0</v>
+      </c>
+      <c r="AB78">
+        <v>0</v>
+      </c>
+      <c r="AC78">
+        <v>0</v>
+      </c>
+      <c r="AD78">
+        <v>0</v>
+      </c>
+      <c r="AE78">
+        <v>0</v>
+      </c>
+      <c r="AF78">
+        <v>0</v>
+      </c>
+      <c r="AG78">
+        <v>1</v>
+      </c>
+      <c r="AH78">
+        <v>1</v>
+      </c>
+      <c r="AJ78">
+        <v>1</v>
+      </c>
+      <c r="AK78">
+        <v>0</v>
+      </c>
+      <c r="AL78">
+        <v>0</v>
+      </c>
+      <c r="AM78">
+        <v>0</v>
+      </c>
+      <c r="AN78">
+        <v>1</v>
+      </c>
+      <c r="AO78">
+        <v>1</v>
+      </c>
+      <c r="AP78">
+        <v>0</v>
+      </c>
+      <c r="AQ78">
+        <v>0</v>
+      </c>
+      <c r="AR78">
+        <v>0</v>
+      </c>
+      <c r="AS78">
+        <v>0</v>
+      </c>
+      <c r="AT78">
+        <v>1</v>
+      </c>
+      <c r="AU78">
+        <v>0</v>
+      </c>
+      <c r="AV78">
+        <v>0</v>
+      </c>
+      <c r="AW78">
+        <v>0</v>
+      </c>
+      <c r="AX78">
+        <v>0</v>
+      </c>
+      <c r="AY78">
+        <v>0</v>
+      </c>
+      <c r="AZ78">
+        <v>0</v>
+      </c>
+      <c r="BA78">
+        <v>0</v>
+      </c>
+      <c r="BB78">
+        <v>0</v>
+      </c>
+      <c r="BC78">
+        <v>1</v>
+      </c>
+      <c r="BD78">
+        <v>1</v>
+      </c>
+      <c r="BE78">
+        <v>0</v>
+      </c>
+      <c r="BF78">
+        <v>0</v>
+      </c>
+      <c r="BG78">
+        <v>0</v>
+      </c>
+      <c r="BH78">
+        <v>0</v>
+      </c>
+      <c r="BI78">
+        <v>0</v>
+      </c>
+      <c r="BJ78">
+        <v>0</v>
+      </c>
+      <c r="BK78">
+        <v>0</v>
+      </c>
+      <c r="BL78">
+        <v>0</v>
+      </c>
+      <c r="BM78">
+        <v>0</v>
+      </c>
+      <c r="BN78">
+        <v>0</v>
+      </c>
+      <c r="BO78">
+        <v>0</v>
+      </c>
+      <c r="BP78">
+        <v>0</v>
+      </c>
+      <c r="BQ78">
+        <v>0</v>
+      </c>
+      <c r="BR78">
+        <v>1</v>
+      </c>
+      <c r="BS78">
+        <v>2</v>
+      </c>
+      <c r="BT78">
+        <v>0</v>
+      </c>
+      <c r="BU78">
+        <v>0</v>
+      </c>
+      <c r="BV78">
+        <v>0</v>
+      </c>
+      <c r="BW78">
+        <v>0</v>
+      </c>
+      <c r="BX78">
+        <v>2</v>
+      </c>
+      <c r="BY78">
+        <v>0</v>
+      </c>
+      <c r="BZ78">
+        <v>4</v>
+      </c>
+      <c r="CA78">
+        <v>1</v>
+      </c>
+      <c r="CB78">
+        <v>0</v>
+      </c>
     </row>
     <row r="79" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A79">
@@ -18460,6 +19381,237 @@
       <c r="C79">
         <v>187</v>
       </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79">
+        <v>1</v>
+      </c>
+      <c r="F79">
+        <v>1</v>
+      </c>
+      <c r="G79">
+        <v>4</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>1</v>
+      </c>
+      <c r="J79">
+        <v>2</v>
+      </c>
+      <c r="K79">
+        <v>1</v>
+      </c>
+      <c r="L79">
+        <v>1</v>
+      </c>
+      <c r="M79">
+        <v>1</v>
+      </c>
+      <c r="N79">
+        <v>0</v>
+      </c>
+      <c r="O79">
+        <v>3</v>
+      </c>
+      <c r="P79">
+        <v>5</v>
+      </c>
+      <c r="Q79">
+        <v>0</v>
+      </c>
+      <c r="R79">
+        <v>3</v>
+      </c>
+      <c r="S79">
+        <v>1</v>
+      </c>
+      <c r="T79">
+        <v>3</v>
+      </c>
+      <c r="U79">
+        <v>2</v>
+      </c>
+      <c r="V79">
+        <v>4</v>
+      </c>
+      <c r="W79">
+        <v>2</v>
+      </c>
+      <c r="X79">
+        <v>0</v>
+      </c>
+      <c r="Y79">
+        <v>4</v>
+      </c>
+      <c r="Z79">
+        <v>1</v>
+      </c>
+      <c r="AA79">
+        <v>1</v>
+      </c>
+      <c r="AB79">
+        <v>1</v>
+      </c>
+      <c r="AC79">
+        <v>2</v>
+      </c>
+      <c r="AD79">
+        <v>1</v>
+      </c>
+      <c r="AE79">
+        <v>7</v>
+      </c>
+      <c r="AF79">
+        <v>2</v>
+      </c>
+      <c r="AG79">
+        <v>2</v>
+      </c>
+      <c r="AH79">
+        <v>6</v>
+      </c>
+      <c r="AI79">
+        <v>6</v>
+      </c>
+      <c r="AJ79">
+        <v>4</v>
+      </c>
+      <c r="AK79">
+        <v>1</v>
+      </c>
+      <c r="AL79">
+        <v>4</v>
+      </c>
+      <c r="AM79">
+        <v>2</v>
+      </c>
+      <c r="AN79">
+        <v>2</v>
+      </c>
+      <c r="AO79">
+        <v>0</v>
+      </c>
+      <c r="AP79">
+        <v>1</v>
+      </c>
+      <c r="AQ79">
+        <v>5</v>
+      </c>
+      <c r="AR79">
+        <v>1</v>
+      </c>
+      <c r="AS79">
+        <v>6</v>
+      </c>
+      <c r="AT79">
+        <v>4</v>
+      </c>
+      <c r="AU79">
+        <v>4</v>
+      </c>
+      <c r="AV79">
+        <v>2</v>
+      </c>
+      <c r="AW79">
+        <v>7</v>
+      </c>
+      <c r="AX79">
+        <v>6</v>
+      </c>
+      <c r="AY79">
+        <v>5</v>
+      </c>
+      <c r="AZ79">
+        <v>7</v>
+      </c>
+      <c r="BA79">
+        <v>6</v>
+      </c>
+      <c r="BB79">
+        <v>4</v>
+      </c>
+      <c r="BC79">
+        <v>4</v>
+      </c>
+      <c r="BD79">
+        <v>6</v>
+      </c>
+      <c r="BE79">
+        <v>1</v>
+      </c>
+      <c r="BF79">
+        <v>0</v>
+      </c>
+      <c r="BG79">
+        <v>0</v>
+      </c>
+      <c r="BH79">
+        <v>0</v>
+      </c>
+      <c r="BI79">
+        <v>0</v>
+      </c>
+      <c r="BJ79">
+        <v>1</v>
+      </c>
+      <c r="BK79">
+        <v>2</v>
+      </c>
+      <c r="BL79">
+        <v>3</v>
+      </c>
+      <c r="BM79">
+        <v>1</v>
+      </c>
+      <c r="BN79">
+        <v>0</v>
+      </c>
+      <c r="BO79">
+        <v>2</v>
+      </c>
+      <c r="BP79">
+        <v>4</v>
+      </c>
+      <c r="BQ79">
+        <v>3</v>
+      </c>
+      <c r="BR79">
+        <v>0</v>
+      </c>
+      <c r="BS79">
+        <v>3</v>
+      </c>
+      <c r="BT79">
+        <v>3</v>
+      </c>
+      <c r="BU79">
+        <v>1</v>
+      </c>
+      <c r="BV79">
+        <v>1</v>
+      </c>
+      <c r="BW79">
+        <v>2</v>
+      </c>
+      <c r="BX79">
+        <v>1</v>
+      </c>
+      <c r="BY79">
+        <v>0</v>
+      </c>
+      <c r="BZ79">
+        <v>4</v>
+      </c>
+      <c r="CA79">
+        <v>4</v>
+      </c>
+      <c r="CB79">
+        <v>1</v>
+      </c>
     </row>
     <row r="80" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A80">
@@ -18946,6 +20098,237 @@
       <c r="C82">
         <v>228</v>
       </c>
+      <c r="D82">
+        <v>4</v>
+      </c>
+      <c r="E82">
+        <v>19</v>
+      </c>
+      <c r="F82">
+        <v>7</v>
+      </c>
+      <c r="G82">
+        <v>5</v>
+      </c>
+      <c r="H82">
+        <v>6</v>
+      </c>
+      <c r="I82">
+        <v>10</v>
+      </c>
+      <c r="J82">
+        <v>5</v>
+      </c>
+      <c r="K82">
+        <v>2</v>
+      </c>
+      <c r="L82">
+        <v>2</v>
+      </c>
+      <c r="M82">
+        <v>3</v>
+      </c>
+      <c r="N82">
+        <v>2</v>
+      </c>
+      <c r="O82">
+        <v>8</v>
+      </c>
+      <c r="P82">
+        <v>3</v>
+      </c>
+      <c r="Q82">
+        <v>4</v>
+      </c>
+      <c r="R82">
+        <v>7</v>
+      </c>
+      <c r="S82">
+        <v>3</v>
+      </c>
+      <c r="T82">
+        <v>2</v>
+      </c>
+      <c r="U82">
+        <v>14</v>
+      </c>
+      <c r="V82">
+        <v>6</v>
+      </c>
+      <c r="W82">
+        <v>7</v>
+      </c>
+      <c r="X82">
+        <v>1</v>
+      </c>
+      <c r="Y82">
+        <v>1</v>
+      </c>
+      <c r="Z82">
+        <v>1</v>
+      </c>
+      <c r="AA82">
+        <v>3</v>
+      </c>
+      <c r="AB82">
+        <v>0</v>
+      </c>
+      <c r="AC82">
+        <v>3</v>
+      </c>
+      <c r="AD82">
+        <v>1</v>
+      </c>
+      <c r="AE82">
+        <v>1</v>
+      </c>
+      <c r="AF82">
+        <v>0</v>
+      </c>
+      <c r="AG82">
+        <v>2</v>
+      </c>
+      <c r="AH82">
+        <v>1</v>
+      </c>
+      <c r="AI82">
+        <v>6</v>
+      </c>
+      <c r="AJ82">
+        <v>1</v>
+      </c>
+      <c r="AK82">
+        <v>0</v>
+      </c>
+      <c r="AL82">
+        <v>1</v>
+      </c>
+      <c r="AM82">
+        <v>10</v>
+      </c>
+      <c r="AN82">
+        <v>5</v>
+      </c>
+      <c r="AO82">
+        <v>0</v>
+      </c>
+      <c r="AP82">
+        <v>0</v>
+      </c>
+      <c r="AQ82">
+        <v>0</v>
+      </c>
+      <c r="AR82">
+        <v>1</v>
+      </c>
+      <c r="AS82">
+        <v>23</v>
+      </c>
+      <c r="AT82">
+        <v>5</v>
+      </c>
+      <c r="AU82">
+        <v>0</v>
+      </c>
+      <c r="AV82">
+        <v>1</v>
+      </c>
+      <c r="AW82">
+        <v>0</v>
+      </c>
+      <c r="AX82">
+        <v>1</v>
+      </c>
+      <c r="AY82">
+        <v>1</v>
+      </c>
+      <c r="AZ82">
+        <v>0</v>
+      </c>
+      <c r="BA82">
+        <v>3</v>
+      </c>
+      <c r="BB82">
+        <v>3</v>
+      </c>
+      <c r="BC82">
+        <v>4</v>
+      </c>
+      <c r="BD82">
+        <v>0</v>
+      </c>
+      <c r="BE82">
+        <v>1</v>
+      </c>
+      <c r="BF82">
+        <v>0</v>
+      </c>
+      <c r="BG82">
+        <v>1</v>
+      </c>
+      <c r="BH82">
+        <v>0</v>
+      </c>
+      <c r="BI82">
+        <v>1</v>
+      </c>
+      <c r="BJ82">
+        <v>1</v>
+      </c>
+      <c r="BK82">
+        <v>4</v>
+      </c>
+      <c r="BL82">
+        <v>0</v>
+      </c>
+      <c r="BM82">
+        <v>0</v>
+      </c>
+      <c r="BN82">
+        <v>2</v>
+      </c>
+      <c r="BO82">
+        <v>1</v>
+      </c>
+      <c r="BP82">
+        <v>1</v>
+      </c>
+      <c r="BQ82">
+        <v>1</v>
+      </c>
+      <c r="BR82">
+        <v>0</v>
+      </c>
+      <c r="BS82">
+        <v>0</v>
+      </c>
+      <c r="BT82">
+        <v>2</v>
+      </c>
+      <c r="BU82">
+        <v>1</v>
+      </c>
+      <c r="BV82">
+        <v>1</v>
+      </c>
+      <c r="BW82">
+        <v>2</v>
+      </c>
+      <c r="BX82">
+        <v>0</v>
+      </c>
+      <c r="BY82">
+        <v>0</v>
+      </c>
+      <c r="BZ82">
+        <v>1</v>
+      </c>
+      <c r="CA82">
+        <v>8</v>
+      </c>
+      <c r="CB82">
+        <v>0</v>
+      </c>
     </row>
     <row r="83" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A83">
@@ -18954,6 +20337,237 @@
       <c r="C83">
         <v>9</v>
       </c>
+      <c r="D83">
+        <v>2</v>
+      </c>
+      <c r="E83">
+        <v>2</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>1</v>
+      </c>
+      <c r="H83">
+        <v>1</v>
+      </c>
+      <c r="I83">
+        <v>1</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+      <c r="K83">
+        <v>0</v>
+      </c>
+      <c r="L83">
+        <v>0</v>
+      </c>
+      <c r="M83">
+        <v>0</v>
+      </c>
+      <c r="N83">
+        <v>0</v>
+      </c>
+      <c r="O83">
+        <v>0</v>
+      </c>
+      <c r="P83">
+        <v>0</v>
+      </c>
+      <c r="Q83">
+        <v>0</v>
+      </c>
+      <c r="R83">
+        <v>0</v>
+      </c>
+      <c r="S83">
+        <v>0</v>
+      </c>
+      <c r="T83">
+        <v>1</v>
+      </c>
+      <c r="U83">
+        <v>0</v>
+      </c>
+      <c r="V83">
+        <v>0</v>
+      </c>
+      <c r="W83">
+        <v>0</v>
+      </c>
+      <c r="X83">
+        <v>0</v>
+      </c>
+      <c r="Y83">
+        <v>0</v>
+      </c>
+      <c r="Z83">
+        <v>0</v>
+      </c>
+      <c r="AA83">
+        <v>0</v>
+      </c>
+      <c r="AB83">
+        <v>1</v>
+      </c>
+      <c r="AC83">
+        <v>0</v>
+      </c>
+      <c r="AD83">
+        <v>0</v>
+      </c>
+      <c r="AE83">
+        <v>0</v>
+      </c>
+      <c r="AF83">
+        <v>0</v>
+      </c>
+      <c r="AG83">
+        <v>0</v>
+      </c>
+      <c r="AH83">
+        <v>0</v>
+      </c>
+      <c r="AI83">
+        <v>0</v>
+      </c>
+      <c r="AJ83">
+        <v>0</v>
+      </c>
+      <c r="AK83">
+        <v>0</v>
+      </c>
+      <c r="AL83">
+        <v>0</v>
+      </c>
+      <c r="AM83">
+        <v>0</v>
+      </c>
+      <c r="AN83">
+        <v>0</v>
+      </c>
+      <c r="AO83">
+        <v>0</v>
+      </c>
+      <c r="AP83">
+        <v>0</v>
+      </c>
+      <c r="AQ83">
+        <v>0</v>
+      </c>
+      <c r="AR83">
+        <v>0</v>
+      </c>
+      <c r="AS83">
+        <v>0</v>
+      </c>
+      <c r="AT83">
+        <v>0</v>
+      </c>
+      <c r="AU83">
+        <v>0</v>
+      </c>
+      <c r="AV83">
+        <v>0</v>
+      </c>
+      <c r="AW83">
+        <v>0</v>
+      </c>
+      <c r="AX83">
+        <v>0</v>
+      </c>
+      <c r="AY83">
+        <v>0</v>
+      </c>
+      <c r="AZ83">
+        <v>0</v>
+      </c>
+      <c r="BA83">
+        <v>0</v>
+      </c>
+      <c r="BB83">
+        <v>0</v>
+      </c>
+      <c r="BC83">
+        <v>0</v>
+      </c>
+      <c r="BD83">
+        <v>0</v>
+      </c>
+      <c r="BE83">
+        <v>0</v>
+      </c>
+      <c r="BF83">
+        <v>0</v>
+      </c>
+      <c r="BG83">
+        <v>0</v>
+      </c>
+      <c r="BH83">
+        <v>0</v>
+      </c>
+      <c r="BI83">
+        <v>0</v>
+      </c>
+      <c r="BJ83">
+        <v>0</v>
+      </c>
+      <c r="BK83">
+        <v>0</v>
+      </c>
+      <c r="BL83">
+        <v>0</v>
+      </c>
+      <c r="BM83">
+        <v>0</v>
+      </c>
+      <c r="BN83">
+        <v>0</v>
+      </c>
+      <c r="BO83">
+        <v>0</v>
+      </c>
+      <c r="BP83">
+        <v>0</v>
+      </c>
+      <c r="BQ83">
+        <v>0</v>
+      </c>
+      <c r="BR83">
+        <v>0</v>
+      </c>
+      <c r="BS83">
+        <v>0</v>
+      </c>
+      <c r="BT83">
+        <v>0</v>
+      </c>
+      <c r="BU83">
+        <v>0</v>
+      </c>
+      <c r="BV83">
+        <v>0</v>
+      </c>
+      <c r="BW83">
+        <v>0</v>
+      </c>
+      <c r="BX83">
+        <v>0</v>
+      </c>
+      <c r="BY83">
+        <v>0</v>
+      </c>
+      <c r="BZ83">
+        <v>0</v>
+      </c>
+      <c r="CA83">
+        <v>0</v>
+      </c>
+      <c r="CB83">
+        <v>0</v>
+      </c>
     </row>
     <row r="84" spans="1:80" x14ac:dyDescent="0.25">
       <c r="A84">
@@ -18961,6 +20575,237 @@
       </c>
       <c r="C84">
         <v>7</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>0</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+      <c r="I84">
+        <v>0</v>
+      </c>
+      <c r="J84">
+        <v>0</v>
+      </c>
+      <c r="K84">
+        <v>0</v>
+      </c>
+      <c r="L84">
+        <v>0</v>
+      </c>
+      <c r="M84">
+        <v>0</v>
+      </c>
+      <c r="N84">
+        <v>0</v>
+      </c>
+      <c r="O84">
+        <v>0</v>
+      </c>
+      <c r="P84">
+        <v>0</v>
+      </c>
+      <c r="Q84">
+        <v>1</v>
+      </c>
+      <c r="R84">
+        <v>3</v>
+      </c>
+      <c r="S84">
+        <v>1</v>
+      </c>
+      <c r="T84">
+        <v>0</v>
+      </c>
+      <c r="U84">
+        <v>0</v>
+      </c>
+      <c r="V84">
+        <v>0</v>
+      </c>
+      <c r="W84">
+        <v>0</v>
+      </c>
+      <c r="X84">
+        <v>0</v>
+      </c>
+      <c r="Y84">
+        <v>0</v>
+      </c>
+      <c r="Z84">
+        <v>0</v>
+      </c>
+      <c r="AA84">
+        <v>0</v>
+      </c>
+      <c r="AB84">
+        <v>0</v>
+      </c>
+      <c r="AC84">
+        <v>0</v>
+      </c>
+      <c r="AD84">
+        <v>0</v>
+      </c>
+      <c r="AE84">
+        <v>0</v>
+      </c>
+      <c r="AF84">
+        <v>0</v>
+      </c>
+      <c r="AG84">
+        <v>0</v>
+      </c>
+      <c r="AH84">
+        <v>0</v>
+      </c>
+      <c r="AI84">
+        <v>2</v>
+      </c>
+      <c r="AJ84">
+        <v>0</v>
+      </c>
+      <c r="AK84">
+        <v>0</v>
+      </c>
+      <c r="AL84">
+        <v>0</v>
+      </c>
+      <c r="AM84">
+        <v>0</v>
+      </c>
+      <c r="AN84">
+        <v>0</v>
+      </c>
+      <c r="AO84">
+        <v>0</v>
+      </c>
+      <c r="AP84">
+        <v>0</v>
+      </c>
+      <c r="AQ84">
+        <v>0</v>
+      </c>
+      <c r="AR84">
+        <v>0</v>
+      </c>
+      <c r="AS84">
+        <v>0</v>
+      </c>
+      <c r="AT84">
+        <v>0</v>
+      </c>
+      <c r="AU84">
+        <v>0</v>
+      </c>
+      <c r="AV84">
+        <v>0</v>
+      </c>
+      <c r="AW84">
+        <v>0</v>
+      </c>
+      <c r="AX84">
+        <v>0</v>
+      </c>
+      <c r="AY84">
+        <v>0</v>
+      </c>
+      <c r="AZ84">
+        <v>0</v>
+      </c>
+      <c r="BA84">
+        <v>0</v>
+      </c>
+      <c r="BB84">
+        <v>0</v>
+      </c>
+      <c r="BC84">
+        <v>0</v>
+      </c>
+      <c r="BD84">
+        <v>0</v>
+      </c>
+      <c r="BE84">
+        <v>0</v>
+      </c>
+      <c r="BF84">
+        <v>0</v>
+      </c>
+      <c r="BG84">
+        <v>0</v>
+      </c>
+      <c r="BH84">
+        <v>0</v>
+      </c>
+      <c r="BI84">
+        <v>0</v>
+      </c>
+      <c r="BJ84">
+        <v>0</v>
+      </c>
+      <c r="BK84">
+        <v>0</v>
+      </c>
+      <c r="BL84">
+        <v>0</v>
+      </c>
+      <c r="BM84">
+        <v>0</v>
+      </c>
+      <c r="BN84">
+        <v>0</v>
+      </c>
+      <c r="BO84">
+        <v>0</v>
+      </c>
+      <c r="BP84">
+        <v>0</v>
+      </c>
+      <c r="BQ84">
+        <v>0</v>
+      </c>
+      <c r="BR84">
+        <v>0</v>
+      </c>
+      <c r="BS84">
+        <v>0</v>
+      </c>
+      <c r="BT84">
+        <v>0</v>
+      </c>
+      <c r="BU84">
+        <v>0</v>
+      </c>
+      <c r="BV84">
+        <v>0</v>
+      </c>
+      <c r="BW84">
+        <v>0</v>
+      </c>
+      <c r="BX84">
+        <v>0</v>
+      </c>
+      <c r="BY84">
+        <v>0</v>
+      </c>
+      <c r="BZ84">
+        <v>0</v>
+      </c>
+      <c r="CA84">
+        <v>0</v>
+      </c>
+      <c r="CB84">
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:80" x14ac:dyDescent="0.25">

</xml_diff>